<commit_message>
generated new hot encodings
</commit_message>
<xml_diff>
--- a/data/formatted/movies_one_hot_encodings.xlsx
+++ b/data/formatted/movies_one_hot_encodings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB134"/>
+  <dimension ref="A1:AC134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,6 +571,11 @@
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
+          <t>imdbRating</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
           <t>BoxOffice</t>
         </is>
       </c>
@@ -660,6 +665,9 @@
         <v>0</v>
       </c>
       <c r="AB2" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="AC2" t="n">
         <v>42629776</v>
       </c>
     </row>
@@ -748,6 +756,9 @@
         <v>0</v>
       </c>
       <c r="AB3" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="AC3" t="n">
         <v>24065925.59677419</v>
       </c>
     </row>
@@ -836,6 +847,9 @@
         <v>0</v>
       </c>
       <c r="AB4" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AC4" t="n">
         <v>20361</v>
       </c>
     </row>
@@ -924,6 +938,9 @@
         <v>0</v>
       </c>
       <c r="AB5" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="AC5" t="n">
         <v>25198598</v>
       </c>
     </row>
@@ -1012,6 +1029,9 @@
         <v>0</v>
       </c>
       <c r="AB6" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="AC6" t="n">
         <v>7251073</v>
       </c>
     </row>
@@ -1100,6 +1120,9 @@
         <v>0</v>
       </c>
       <c r="AB7" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="AC7" t="n">
         <v>38493</v>
       </c>
     </row>
@@ -1188,6 +1211,9 @@
         <v>0</v>
       </c>
       <c r="AB8" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AC8" t="n">
         <v>115171585</v>
       </c>
     </row>
@@ -1276,6 +1302,9 @@
         <v>0</v>
       </c>
       <c r="AB9" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AC9" t="n">
         <v>64065</v>
       </c>
     </row>
@@ -1364,6 +1393,9 @@
         <v>0</v>
       </c>
       <c r="AB10" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AC10" t="n">
         <v>1110707</v>
       </c>
     </row>
@@ -1452,6 +1484,9 @@
         <v>0</v>
       </c>
       <c r="AB11" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AC11" t="n">
         <v>56629811.40740741</v>
       </c>
     </row>
@@ -1540,6 +1575,9 @@
         <v>0</v>
       </c>
       <c r="AB12" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="AC12" t="n">
         <v>62524260</v>
       </c>
     </row>
@@ -1628,6 +1666,9 @@
         <v>0</v>
       </c>
       <c r="AB13" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="AC13" t="n">
         <v>2964845</v>
       </c>
     </row>
@@ -1716,6 +1757,9 @@
         <v>0</v>
       </c>
       <c r="AB14" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AC14" t="n">
         <v>90570999</v>
       </c>
     </row>
@@ -1804,6 +1848,9 @@
         <v>0</v>
       </c>
       <c r="AB15" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="AC15" t="n">
         <v>40456565</v>
       </c>
     </row>
@@ -1892,6 +1939,9 @@
         <v>0</v>
       </c>
       <c r="AB16" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="AC16" t="n">
         <v>188024361</v>
       </c>
     </row>
@@ -1980,6 +2030,9 @@
         <v>0</v>
       </c>
       <c r="AB17" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="AC17" t="n">
         <v>20774575</v>
       </c>
     </row>
@@ -2068,6 +2121,9 @@
         <v>0</v>
       </c>
       <c r="AB18" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AC18" t="n">
         <v>4886216</v>
       </c>
     </row>
@@ -2156,6 +2212,9 @@
         <v>0</v>
       </c>
       <c r="AB19" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC19" t="n">
         <v>872142</v>
       </c>
     </row>
@@ -2244,6 +2303,9 @@
         <v>0</v>
       </c>
       <c r="AB20" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC20" t="n">
         <v>4631</v>
       </c>
     </row>
@@ -2332,6 +2394,9 @@
         <v>0</v>
       </c>
       <c r="AB21" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="AC21" t="n">
         <v>267263625</v>
       </c>
     </row>
@@ -2420,6 +2485,9 @@
         <v>0</v>
       </c>
       <c r="AB22" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AC22" t="n">
         <v>21756163</v>
       </c>
     </row>
@@ -2508,6 +2576,9 @@
         <v>0</v>
       </c>
       <c r="AB23" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="AC23" t="n">
         <v>754301</v>
       </c>
     </row>
@@ -2596,6 +2667,9 @@
         <v>0</v>
       </c>
       <c r="AB24" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="AC24" t="n">
         <v>4059680</v>
       </c>
     </row>
@@ -2684,6 +2758,9 @@
         <v>0</v>
       </c>
       <c r="AB25" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC25" t="n">
         <v>3765585</v>
       </c>
     </row>
@@ -2772,6 +2849,9 @@
         <v>0</v>
       </c>
       <c r="AB26" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="AC26" t="n">
         <v>872256</v>
       </c>
     </row>
@@ -2860,6 +2940,9 @@
         <v>0</v>
       </c>
       <c r="AB27" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC27" t="n">
         <v>57377916</v>
       </c>
     </row>
@@ -2948,6 +3031,9 @@
         <v>0</v>
       </c>
       <c r="AB28" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AC28" t="n">
         <v>167510016</v>
       </c>
     </row>
@@ -3036,6 +3122,9 @@
         <v>0</v>
       </c>
       <c r="AB29" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="AC29" t="n">
         <v>24668669</v>
       </c>
     </row>
@@ -3124,6 +3213,9 @@
         <v>0</v>
       </c>
       <c r="AB30" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AC30" t="n">
         <v>12803305</v>
       </c>
     </row>
@@ -3212,6 +3304,9 @@
         <v>0</v>
       </c>
       <c r="AB31" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC31" t="n">
         <v>24065925.59677419</v>
       </c>
     </row>
@@ -3300,6 +3395,9 @@
         <v>0</v>
       </c>
       <c r="AB32" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC32" t="n">
         <v>24065925.59677419</v>
       </c>
     </row>
@@ -3388,6 +3486,9 @@
         <v>0</v>
       </c>
       <c r="AB33" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="AC33" t="n">
         <v>5778353</v>
       </c>
     </row>
@@ -3476,6 +3577,9 @@
         <v>0</v>
       </c>
       <c r="AB34" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="AC34" t="n">
         <v>443684</v>
       </c>
     </row>
@@ -3564,6 +3668,9 @@
         <v>0</v>
       </c>
       <c r="AB35" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="AC35" t="n">
         <v>38493</v>
       </c>
     </row>
@@ -3652,6 +3759,9 @@
         <v>0</v>
       </c>
       <c r="AB36" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC36" t="n">
         <v>41263140</v>
       </c>
     </row>
@@ -3740,6 +3850,9 @@
         <v>0</v>
       </c>
       <c r="AB37" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="AC37" t="n">
         <v>14481606</v>
       </c>
     </row>
@@ -3828,6 +3941,9 @@
         <v>0</v>
       </c>
       <c r="AB38" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AC38" t="n">
         <v>2410914</v>
       </c>
     </row>
@@ -3916,6 +4032,9 @@
         <v>0</v>
       </c>
       <c r="AB39" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AC39" t="n">
         <v>38122883</v>
       </c>
     </row>
@@ -4004,6 +4123,9 @@
         <v>0</v>
       </c>
       <c r="AB40" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="AC40" t="n">
         <v>56629811.40740741</v>
       </c>
     </row>
@@ -4092,6 +4214,9 @@
         <v>0</v>
       </c>
       <c r="AB41" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="AC41" t="n">
         <v>38016380</v>
       </c>
     </row>
@@ -4180,6 +4305,9 @@
         <v>0</v>
       </c>
       <c r="AB42" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AC42" t="n">
         <v>21218403</v>
       </c>
     </row>
@@ -4268,6 +4396,9 @@
         <v>0</v>
       </c>
       <c r="AB43" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="AC43" t="n">
         <v>12811858</v>
       </c>
     </row>
@@ -4356,6 +4487,9 @@
         <v>0</v>
       </c>
       <c r="AB44" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="AC44" t="n">
         <v>969869</v>
       </c>
     </row>
@@ -4444,6 +4578,9 @@
         <v>0</v>
       </c>
       <c r="AB45" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC45" t="n">
         <v>1087585</v>
       </c>
     </row>
@@ -4532,6 +4669,9 @@
         <v>0</v>
       </c>
       <c r="AB46" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="AC46" t="n">
         <v>81903458</v>
       </c>
     </row>
@@ -4620,6 +4760,9 @@
         <v>0</v>
       </c>
       <c r="AB47" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="AC47" t="n">
         <v>36850101</v>
       </c>
     </row>
@@ -4708,6 +4851,9 @@
         <v>0</v>
       </c>
       <c r="AB48" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AC48" t="n">
         <v>24650296</v>
       </c>
     </row>
@@ -4796,6 +4942,9 @@
         <v>0</v>
       </c>
       <c r="AB49" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AC49" t="n">
         <v>130444603</v>
       </c>
     </row>
@@ -4884,6 +5033,9 @@
         <v>1</v>
       </c>
       <c r="AB50" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AC50" t="n">
         <v>12423831</v>
       </c>
     </row>
@@ -4972,6 +5124,9 @@
         <v>0</v>
       </c>
       <c r="AB51" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC51" t="n">
         <v>65075540</v>
       </c>
     </row>
@@ -5060,6 +5215,9 @@
         <v>0</v>
       </c>
       <c r="AB52" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AC52" t="n">
         <v>38493</v>
       </c>
     </row>
@@ -5148,6 +5306,9 @@
         <v>0</v>
       </c>
       <c r="AB53" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC53" t="n">
         <v>110101975</v>
       </c>
     </row>
@@ -5236,6 +5397,9 @@
         <v>0</v>
       </c>
       <c r="AB54" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC54" t="n">
         <v>20324096</v>
       </c>
     </row>
@@ -5324,6 +5488,9 @@
         <v>0</v>
       </c>
       <c r="AB55" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC55" t="n">
         <v>56629811.40740741</v>
       </c>
     </row>
@@ -5412,6 +5579,9 @@
         <v>0</v>
       </c>
       <c r="AB56" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="AC56" t="n">
         <v>24065925.59677419</v>
       </c>
     </row>
@@ -5500,6 +5670,9 @@
         <v>0</v>
       </c>
       <c r="AB57" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="AC57" t="n">
         <v>83301580</v>
       </c>
     </row>
@@ -5588,6 +5761,9 @@
         <v>0</v>
       </c>
       <c r="AB58" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AC58" t="n">
         <v>3581642</v>
       </c>
     </row>
@@ -5676,6 +5852,9 @@
         <v>0</v>
       </c>
       <c r="AB59" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AC59" t="n">
         <v>10763520</v>
       </c>
     </row>
@@ -5764,6 +5943,9 @@
         <v>0</v>
       </c>
       <c r="AB60" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AC60" t="n">
         <v>38493</v>
       </c>
     </row>
@@ -5852,6 +6034,9 @@
         <v>0</v>
       </c>
       <c r="AB61" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="AC61" t="n">
         <v>35291068</v>
       </c>
     </row>
@@ -5940,6 +6125,9 @@
         <v>0</v>
       </c>
       <c r="AB62" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="AC62" t="n">
         <v>63686397</v>
       </c>
     </row>
@@ -6028,6 +6216,9 @@
         <v>0</v>
       </c>
       <c r="AB63" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="AC63" t="n">
         <v>85364450</v>
       </c>
     </row>
@@ -6116,6 +6307,9 @@
         <v>0</v>
       </c>
       <c r="AB64" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AC64" t="n">
         <v>38493</v>
       </c>
     </row>
@@ -6204,6 +6398,9 @@
         <v>0</v>
       </c>
       <c r="AB65" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="AC65" t="n">
         <v>45512466</v>
       </c>
     </row>
@@ -6292,6 +6489,9 @@
         <v>0</v>
       </c>
       <c r="AB66" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="AC66" t="n">
         <v>132399394</v>
       </c>
     </row>
@@ -6380,6 +6580,9 @@
         <v>0</v>
       </c>
       <c r="AB67" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="AC67" t="n">
         <v>12134935</v>
       </c>
     </row>
@@ -6468,6 +6671,9 @@
         <v>0</v>
       </c>
       <c r="AB68" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="AC68" t="n">
         <v>17300439</v>
       </c>
     </row>
@@ -6556,6 +6762,9 @@
         <v>0</v>
       </c>
       <c r="AB69" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AC69" t="n">
         <v>35857181</v>
       </c>
     </row>
@@ -6644,6 +6853,9 @@
         <v>0</v>
       </c>
       <c r="AB70" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="AC70" t="n">
         <v>26302731</v>
       </c>
     </row>
@@ -6732,6 +6944,9 @@
         <v>0</v>
       </c>
       <c r="AB71" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="AC71" t="n">
         <v>15472775</v>
       </c>
     </row>
@@ -6820,6 +7035,9 @@
         <v>0</v>
       </c>
       <c r="AB72" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="AC72" t="n">
         <v>13303319</v>
       </c>
     </row>
@@ -6908,6 +7126,9 @@
         <v>0</v>
       </c>
       <c r="AB73" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC73" t="n">
         <v>52767889</v>
       </c>
     </row>
@@ -6996,6 +7217,9 @@
         <v>0</v>
       </c>
       <c r="AB74" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="AC74" t="n">
         <v>221805</v>
       </c>
     </row>
@@ -7084,6 +7308,9 @@
         <v>0</v>
       </c>
       <c r="AB75" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC75" t="n">
         <v>24065925.59677419</v>
       </c>
     </row>
@@ -7172,6 +7399,9 @@
         <v>0</v>
       </c>
       <c r="AB76" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="AC76" t="n">
         <v>11603545</v>
       </c>
     </row>
@@ -7260,6 +7490,9 @@
         <v>0</v>
       </c>
       <c r="AB77" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="AC77" t="n">
         <v>44806783</v>
       </c>
     </row>
@@ -7348,6 +7581,9 @@
         <v>0</v>
       </c>
       <c r="AB78" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC78" t="n">
         <v>62950384</v>
       </c>
     </row>
@@ -7436,6 +7672,9 @@
         <v>0</v>
       </c>
       <c r="AB79" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AC79" t="n">
         <v>24065925.59677419</v>
       </c>
     </row>
@@ -7524,6 +7763,9 @@
         <v>0</v>
       </c>
       <c r="AB80" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="AC80" t="n">
         <v>101196</v>
       </c>
     </row>
@@ -7612,6 +7854,9 @@
         <v>0</v>
       </c>
       <c r="AB81" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AC81" t="n">
         <v>12482775</v>
       </c>
     </row>
@@ -7700,6 +7945,9 @@
         <v>0</v>
       </c>
       <c r="AB82" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AC82" t="n">
         <v>213307889</v>
       </c>
     </row>
@@ -7788,6 +8036,9 @@
         <v>0</v>
       </c>
       <c r="AB83" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AC83" t="n">
         <v>25785603</v>
       </c>
     </row>
@@ -7876,6 +8127,9 @@
         <v>0</v>
       </c>
       <c r="AB84" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="AC84" t="n">
         <v>30610863</v>
       </c>
     </row>
@@ -7964,6 +8218,9 @@
         <v>0</v>
       </c>
       <c r="AB85" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="AC85" t="n">
         <v>128505958</v>
       </c>
     </row>
@@ -8052,6 +8309,9 @@
         <v>0</v>
       </c>
       <c r="AB86" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="AC86" t="n">
         <v>24065925.59677419</v>
       </c>
     </row>
@@ -8140,6 +8400,9 @@
         <v>0</v>
       </c>
       <c r="AB87" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC87" t="n">
         <v>1132112</v>
       </c>
     </row>
@@ -8228,6 +8491,9 @@
         <v>0</v>
       </c>
       <c r="AB88" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="AC88" t="n">
         <v>4211129</v>
       </c>
     </row>
@@ -8316,6 +8582,9 @@
         <v>0</v>
       </c>
       <c r="AB89" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="AC89" t="n">
         <v>70958</v>
       </c>
     </row>
@@ -8404,6 +8673,9 @@
         <v>0</v>
       </c>
       <c r="AB90" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AC90" t="n">
         <v>591366</v>
       </c>
     </row>
@@ -8492,6 +8764,9 @@
         <v>0</v>
       </c>
       <c r="AB91" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC91" t="n">
         <v>20763013</v>
       </c>
     </row>
@@ -8580,6 +8855,9 @@
         <v>0</v>
       </c>
       <c r="AB92" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="AC92" t="n">
         <v>24065925.59677419</v>
       </c>
     </row>
@@ -8668,6 +8946,9 @@
         <v>0</v>
       </c>
       <c r="AB93" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC93" t="n">
         <v>50000000</v>
       </c>
     </row>
@@ -8756,6 +9037,9 @@
         <v>0</v>
       </c>
       <c r="AB94" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="AC94" t="n">
         <v>3909002</v>
       </c>
     </row>
@@ -8844,6 +9128,9 @@
         <v>0</v>
       </c>
       <c r="AB95" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC95" t="n">
         <v>160861908</v>
       </c>
     </row>
@@ -8932,6 +9219,9 @@
         <v>0</v>
       </c>
       <c r="AB96" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="AC96" t="n">
         <v>54766923</v>
       </c>
     </row>
@@ -9020,6 +9310,9 @@
         <v>0</v>
       </c>
       <c r="AB97" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC97" t="n">
         <v>261441092</v>
       </c>
     </row>
@@ -9108,6 +9401,9 @@
         <v>0</v>
       </c>
       <c r="AB98" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AC98" t="n">
         <v>56629811.40740741</v>
       </c>
     </row>
@@ -9196,6 +9492,9 @@
         <v>0</v>
       </c>
       <c r="AB99" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="AC99" t="n">
         <v>243640120</v>
       </c>
     </row>
@@ -9284,6 +9583,9 @@
         <v>0</v>
       </c>
       <c r="AB100" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AC100" t="n">
         <v>46236000</v>
       </c>
     </row>
@@ -9372,6 +9674,9 @@
         <v>0</v>
       </c>
       <c r="AB101" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="AC101" t="n">
         <v>58715510</v>
       </c>
     </row>
@@ -9460,6 +9765,9 @@
         <v>0</v>
       </c>
       <c r="AB102" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="AC102" t="n">
         <v>30212620</v>
       </c>
     </row>
@@ -9548,6 +9856,9 @@
         <v>0</v>
       </c>
       <c r="AB103" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="AC103" t="n">
         <v>560069</v>
       </c>
     </row>
@@ -9636,6 +9947,9 @@
         <v>0</v>
       </c>
       <c r="AB104" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AC104" t="n">
         <v>155019340</v>
       </c>
     </row>
@@ -9724,6 +10038,9 @@
         <v>0</v>
       </c>
       <c r="AB105" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="AC105" t="n">
         <v>49438370</v>
       </c>
     </row>
@@ -9812,6 +10129,9 @@
         <v>0</v>
       </c>
       <c r="AB106" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="AC106" t="n">
         <v>61123569</v>
       </c>
     </row>
@@ -9900,6 +10220,9 @@
         <v>0</v>
       </c>
       <c r="AB107" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC107" t="n">
         <v>93953653</v>
       </c>
     </row>
@@ -9988,6 +10311,9 @@
         <v>0</v>
       </c>
       <c r="AB108" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AC108" t="n">
         <v>140125968</v>
       </c>
     </row>
@@ -10076,6 +10402,9 @@
         <v>0</v>
       </c>
       <c r="AB109" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AC109" t="n">
         <v>3242457</v>
       </c>
     </row>
@@ -10164,6 +10493,9 @@
         <v>0</v>
       </c>
       <c r="AB110" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="AC110" t="n">
         <v>245852179</v>
       </c>
     </row>
@@ -10252,6 +10584,9 @@
         <v>0</v>
       </c>
       <c r="AB111" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC111" t="n">
         <v>42313354</v>
       </c>
     </row>
@@ -10340,6 +10675,9 @@
         <v>0</v>
       </c>
       <c r="AB112" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="AC112" t="n">
         <v>3263585</v>
       </c>
     </row>
@@ -10428,6 +10766,9 @@
         <v>0</v>
       </c>
       <c r="AB113" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC113" t="n">
         <v>18119640</v>
       </c>
     </row>
@@ -10516,6 +10857,9 @@
         <v>0</v>
       </c>
       <c r="AB114" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC114" t="n">
         <v>55474756</v>
       </c>
     </row>
@@ -10604,6 +10948,9 @@
         <v>0</v>
       </c>
       <c r="AB115" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="AC115" t="n">
         <v>14915773</v>
       </c>
     </row>
@@ -10692,6 +11039,9 @@
         <v>0</v>
       </c>
       <c r="AB116" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="AC116" t="n">
         <v>102247150</v>
       </c>
     </row>
@@ -10780,6 +11130,9 @@
         <v>0</v>
       </c>
       <c r="AB117" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="AC117" t="n">
         <v>70136369</v>
       </c>
     </row>
@@ -10868,6 +11221,9 @@
         <v>0</v>
       </c>
       <c r="AB118" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC118" t="n">
         <v>60106536</v>
       </c>
     </row>
@@ -10956,6 +11312,9 @@
         <v>0</v>
       </c>
       <c r="AB119" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="AC119" t="n">
         <v>13167232</v>
       </c>
     </row>
@@ -11044,6 +11403,9 @@
         <v>0</v>
       </c>
       <c r="AB120" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="AC120" t="n">
         <v>2832029</v>
       </c>
     </row>
@@ -11132,6 +11494,9 @@
         <v>0</v>
       </c>
       <c r="AB121" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="AC121" t="n">
         <v>316472</v>
       </c>
     </row>
@@ -11220,6 +11585,9 @@
         <v>0</v>
       </c>
       <c r="AB122" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="AC122" t="n">
         <v>33479698</v>
       </c>
     </row>
@@ -11308,6 +11676,9 @@
         <v>0</v>
       </c>
       <c r="AB123" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="AC123" t="n">
         <v>7266383</v>
       </c>
     </row>
@@ -11396,6 +11767,9 @@
         <v>0</v>
       </c>
       <c r="AB124" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="AC124" t="n">
         <v>236452</v>
       </c>
     </row>
@@ -11484,6 +11858,9 @@
         <v>0</v>
       </c>
       <c r="AB125" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="AC125" t="n">
         <v>67436818</v>
       </c>
     </row>
@@ -11572,6 +11949,9 @@
         <v>0</v>
       </c>
       <c r="AB126" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="AC126" t="n">
         <v>2201923</v>
       </c>
     </row>
@@ -11660,6 +12040,9 @@
         <v>0</v>
       </c>
       <c r="AB127" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="AC127" t="n">
         <v>38493</v>
       </c>
     </row>
@@ -11748,6 +12131,9 @@
         <v>0</v>
       </c>
       <c r="AB128" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="AC128" t="n">
         <v>7434726</v>
       </c>
     </row>
@@ -11836,6 +12222,9 @@
         <v>0</v>
       </c>
       <c r="AB129" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="AC129" t="n">
         <v>2678691</v>
       </c>
     </row>
@@ -11924,6 +12313,9 @@
         <v>0</v>
       </c>
       <c r="AB130" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="AC130" t="n">
         <v>17323326</v>
       </c>
     </row>
@@ -12012,6 +12404,9 @@
         <v>0</v>
       </c>
       <c r="AB131" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="AC131" t="n">
         <v>1730597</v>
       </c>
     </row>
@@ -12100,6 +12495,9 @@
         <v>0</v>
       </c>
       <c r="AB132" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AC132" t="n">
         <v>219964115</v>
       </c>
     </row>
@@ -12188,6 +12586,9 @@
         <v>0</v>
       </c>
       <c r="AB133" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AC133" t="n">
         <v>14377198</v>
       </c>
     </row>
@@ -12275,7 +12676,10 @@
       <c r="AA134" t="n">
         <v>0</v>
       </c>
-      <c r="AB134" t="inlineStr"/>
+      <c r="AB134" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="AC134" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
generated data with trends
</commit_message>
<xml_diff>
--- a/data/formatted/movies_one_hot_encodings.xlsx
+++ b/data/formatted/movies_one_hot_encodings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC134"/>
+  <dimension ref="A1:AD134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,35 +546,40 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
+          <t>Search Trend</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
           <t>PG-13</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Unrated</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>PG</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>NC-17</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Approved</t>
         </is>
@@ -650,10 +655,10 @@
         <v>42629776</v>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>1068</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -668,6 +673,9 @@
         <v>0</v>
       </c>
       <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -740,14 +748,12 @@
       <c r="V3" t="n">
         <v>24065925.59677419</v>
       </c>
-      <c r="W3" t="n">
-        <v>0</v>
-      </c>
+      <c r="W3" t="inlineStr"/>
       <c r="X3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3" t="n">
         <v>0</v>
@@ -759,6 +765,9 @@
         <v>0</v>
       </c>
       <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -831,14 +840,12 @@
       <c r="V4" t="n">
         <v>20361</v>
       </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
+      <c r="W4" t="inlineStr"/>
       <c r="X4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4" t="n">
         <v>0</v>
@@ -850,6 +857,9 @@
         <v>0</v>
       </c>
       <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -922,14 +932,12 @@
       <c r="V5" t="n">
         <v>25198598</v>
       </c>
-      <c r="W5" t="n">
-        <v>0</v>
-      </c>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" t="n">
         <v>0</v>
@@ -941,6 +949,9 @@
         <v>0</v>
       </c>
       <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1014,13 +1025,13 @@
         <v>7251073</v>
       </c>
       <c r="W6" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="X6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" t="n">
         <v>0</v>
@@ -1032,6 +1043,9 @@
         <v>0</v>
       </c>
       <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1104,17 +1118,15 @@
       <c r="V7" t="n">
         <v>455317.5</v>
       </c>
-      <c r="W7" t="n">
-        <v>0</v>
-      </c>
+      <c r="W7" t="inlineStr"/>
       <c r="X7" t="n">
         <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
@@ -1123,6 +1135,9 @@
         <v>0</v>
       </c>
       <c r="AC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1196,13 +1211,13 @@
         <v>115171585</v>
       </c>
       <c r="W8" t="n">
-        <v>0</v>
+        <v>421</v>
       </c>
       <c r="X8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
@@ -1214,6 +1229,9 @@
         <v>0</v>
       </c>
       <c r="AC8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1287,13 +1305,13 @@
         <v>64065</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="X9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9" t="n">
         <v>0</v>
@@ -1305,6 +1323,9 @@
         <v>0</v>
       </c>
       <c r="AC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1378,13 +1399,13 @@
         <v>1110707</v>
       </c>
       <c r="W10" t="n">
-        <v>0</v>
+        <v>2770</v>
       </c>
       <c r="X10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10" t="n">
         <v>0</v>
@@ -1396,6 +1417,9 @@
         <v>0</v>
       </c>
       <c r="AC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1469,10 +1493,10 @@
         <v>56629811.40740741</v>
       </c>
       <c r="W11" t="n">
-        <v>1</v>
+        <v>333</v>
       </c>
       <c r="X11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" t="n">
         <v>0</v>
@@ -1487,6 +1511,9 @@
         <v>0</v>
       </c>
       <c r="AC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1560,13 +1587,13 @@
         <v>62524260</v>
       </c>
       <c r="W12" t="n">
-        <v>0</v>
+        <v>856</v>
       </c>
       <c r="X12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12" t="n">
         <v>0</v>
@@ -1578,6 +1605,9 @@
         <v>0</v>
       </c>
       <c r="AC12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1651,13 +1681,13 @@
         <v>2964845</v>
       </c>
       <c r="W13" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="X13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13" t="n">
         <v>0</v>
@@ -1669,6 +1699,9 @@
         <v>0</v>
       </c>
       <c r="AC13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1741,14 +1774,12 @@
       <c r="V14" t="n">
         <v>90570999</v>
       </c>
-      <c r="W14" t="n">
-        <v>0</v>
-      </c>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14" t="n">
         <v>0</v>
@@ -1760,6 +1791,9 @@
         <v>0</v>
       </c>
       <c r="AC14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1832,14 +1866,12 @@
       <c r="V15" t="n">
         <v>40456565</v>
       </c>
-      <c r="W15" t="n">
-        <v>0</v>
-      </c>
+      <c r="W15" t="inlineStr"/>
       <c r="X15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15" t="n">
         <v>0</v>
@@ -1851,6 +1883,9 @@
         <v>0</v>
       </c>
       <c r="AC15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1924,10 +1959,10 @@
         <v>188024361</v>
       </c>
       <c r="W16" t="n">
-        <v>1</v>
+        <v>638</v>
       </c>
       <c r="X16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" t="n">
         <v>0</v>
@@ -1942,6 +1977,9 @@
         <v>0</v>
       </c>
       <c r="AC16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2015,7 +2053,7 @@
         <v>20774575</v>
       </c>
       <c r="W17" t="n">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -2024,15 +2062,18 @@
         <v>0</v>
       </c>
       <c r="Z17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB17" t="n">
         <v>0</v>
       </c>
       <c r="AC17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2105,14 +2146,12 @@
       <c r="V18" t="n">
         <v>4886216</v>
       </c>
-      <c r="W18" t="n">
-        <v>0</v>
-      </c>
+      <c r="W18" t="inlineStr"/>
       <c r="X18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z18" t="n">
         <v>0</v>
@@ -2124,6 +2163,9 @@
         <v>0</v>
       </c>
       <c r="AC18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2196,17 +2238,15 @@
       <c r="V19" t="n">
         <v>872142</v>
       </c>
-      <c r="W19" t="n">
-        <v>0</v>
-      </c>
+      <c r="W19" t="inlineStr"/>
       <c r="X19" t="n">
         <v>0</v>
       </c>
       <c r="Y19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA19" t="n">
         <v>0</v>
@@ -2215,6 +2255,9 @@
         <v>0</v>
       </c>
       <c r="AC19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2288,13 +2331,13 @@
         <v>4631</v>
       </c>
       <c r="W20" t="n">
-        <v>0</v>
+        <v>866</v>
       </c>
       <c r="X20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z20" t="n">
         <v>0</v>
@@ -2306,6 +2349,9 @@
         <v>0</v>
       </c>
       <c r="AC20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2378,9 +2424,7 @@
       <c r="V21" t="n">
         <v>267263625</v>
       </c>
-      <c r="W21" t="n">
-        <v>0</v>
-      </c>
+      <c r="W21" t="inlineStr"/>
       <c r="X21" t="n">
         <v>0</v>
       </c>
@@ -2388,15 +2432,18 @@
         <v>0</v>
       </c>
       <c r="Z21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB21" t="n">
         <v>0</v>
       </c>
       <c r="AC21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2469,14 +2516,12 @@
       <c r="V22" t="n">
         <v>21756163</v>
       </c>
-      <c r="W22" t="n">
-        <v>0</v>
-      </c>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z22" t="n">
         <v>0</v>
@@ -2488,6 +2533,9 @@
         <v>0</v>
       </c>
       <c r="AC22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2561,13 +2609,13 @@
         <v>754301</v>
       </c>
       <c r="W23" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="X23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z23" t="n">
         <v>0</v>
@@ -2579,6 +2627,9 @@
         <v>0</v>
       </c>
       <c r="AC23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2651,14 +2702,12 @@
       <c r="V24" t="n">
         <v>4059680</v>
       </c>
-      <c r="W24" t="n">
-        <v>0</v>
-      </c>
+      <c r="W24" t="inlineStr"/>
       <c r="X24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z24" t="n">
         <v>0</v>
@@ -2670,6 +2719,9 @@
         <v>0</v>
       </c>
       <c r="AC24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2742,14 +2794,12 @@
       <c r="V25" t="n">
         <v>3765585</v>
       </c>
-      <c r="W25" t="n">
-        <v>0</v>
-      </c>
+      <c r="W25" t="inlineStr"/>
       <c r="X25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z25" t="n">
         <v>0</v>
@@ -2761,6 +2811,9 @@
         <v>0</v>
       </c>
       <c r="AC25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2833,14 +2886,12 @@
       <c r="V26" t="n">
         <v>872256</v>
       </c>
-      <c r="W26" t="n">
-        <v>0</v>
-      </c>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" t="n">
         <v>0</v>
@@ -2852,6 +2903,9 @@
         <v>0</v>
       </c>
       <c r="AC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2924,14 +2978,12 @@
       <c r="V27" t="n">
         <v>57377916</v>
       </c>
-      <c r="W27" t="n">
-        <v>0</v>
-      </c>
+      <c r="W27" t="inlineStr"/>
       <c r="X27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z27" t="n">
         <v>0</v>
@@ -2943,6 +2995,9 @@
         <v>0</v>
       </c>
       <c r="AC27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3025,15 +3080,18 @@
         <v>0</v>
       </c>
       <c r="Z28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB28" t="n">
         <v>0</v>
       </c>
       <c r="AC28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3106,9 +3164,7 @@
       <c r="V29" t="n">
         <v>24668669</v>
       </c>
-      <c r="W29" t="n">
-        <v>0</v>
-      </c>
+      <c r="W29" t="inlineStr"/>
       <c r="X29" t="n">
         <v>0</v>
       </c>
@@ -3119,12 +3175,15 @@
         <v>0</v>
       </c>
       <c r="AA29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3197,11 +3256,9 @@
       <c r="V30" t="n">
         <v>12803305</v>
       </c>
-      <c r="W30" t="n">
-        <v>1</v>
-      </c>
+      <c r="W30" t="inlineStr"/>
       <c r="X30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y30" t="n">
         <v>0</v>
@@ -3216,6 +3273,9 @@
         <v>0</v>
       </c>
       <c r="AC30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3289,13 +3349,13 @@
         <v>24065925.59677419</v>
       </c>
       <c r="W31" t="n">
-        <v>0</v>
+        <v>1025</v>
       </c>
       <c r="X31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z31" t="n">
         <v>0</v>
@@ -3307,6 +3367,9 @@
         <v>0</v>
       </c>
       <c r="AC31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3380,13 +3443,13 @@
         <v>24065925.59677419</v>
       </c>
       <c r="W32" t="n">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="X32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z32" t="n">
         <v>0</v>
@@ -3398,6 +3461,9 @@
         <v>0</v>
       </c>
       <c r="AC32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3470,9 +3536,7 @@
       <c r="V33" t="n">
         <v>5778353</v>
       </c>
-      <c r="W33" t="n">
-        <v>0</v>
-      </c>
+      <c r="W33" t="inlineStr"/>
       <c r="X33" t="n">
         <v>0</v>
       </c>
@@ -3480,15 +3544,18 @@
         <v>0</v>
       </c>
       <c r="Z33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB33" t="n">
         <v>0</v>
       </c>
       <c r="AC33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3562,13 +3629,13 @@
         <v>443684</v>
       </c>
       <c r="W34" t="n">
-        <v>0</v>
+        <v>4785</v>
       </c>
       <c r="X34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z34" t="n">
         <v>0</v>
@@ -3580,6 +3647,9 @@
         <v>0</v>
       </c>
       <c r="AC34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3653,16 +3723,16 @@
         <v>455317.5</v>
       </c>
       <c r="W35" t="n">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="X35" t="n">
         <v>0</v>
       </c>
       <c r="Y35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA35" t="n">
         <v>0</v>
@@ -3671,6 +3741,9 @@
         <v>0</v>
       </c>
       <c r="AC35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3743,14 +3816,12 @@
       <c r="V36" t="n">
         <v>41263140</v>
       </c>
-      <c r="W36" t="n">
-        <v>0</v>
-      </c>
+      <c r="W36" t="inlineStr"/>
       <c r="X36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z36" t="n">
         <v>0</v>
@@ -3762,6 +3833,9 @@
         <v>0</v>
       </c>
       <c r="AC36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3834,14 +3908,12 @@
       <c r="V37" t="n">
         <v>14481606</v>
       </c>
-      <c r="W37" t="n">
-        <v>0</v>
-      </c>
+      <c r="W37" t="inlineStr"/>
       <c r="X37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z37" t="n">
         <v>0</v>
@@ -3853,6 +3925,9 @@
         <v>0</v>
       </c>
       <c r="AC37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3926,13 +4001,13 @@
         <v>2410914</v>
       </c>
       <c r="W38" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="X38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z38" t="n">
         <v>0</v>
@@ -3944,6 +4019,9 @@
         <v>0</v>
       </c>
       <c r="AC38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4017,13 +4095,13 @@
         <v>38122883</v>
       </c>
       <c r="W39" t="n">
-        <v>0</v>
+        <v>628</v>
       </c>
       <c r="X39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z39" t="n">
         <v>0</v>
@@ -4035,6 +4113,9 @@
         <v>0</v>
       </c>
       <c r="AC39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4108,10 +4189,10 @@
         <v>56629811.40740741</v>
       </c>
       <c r="W40" t="n">
-        <v>1</v>
+        <v>259</v>
       </c>
       <c r="X40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y40" t="n">
         <v>0</v>
@@ -4126,6 +4207,9 @@
         <v>0</v>
       </c>
       <c r="AC40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4198,14 +4282,12 @@
       <c r="V41" t="n">
         <v>38016380</v>
       </c>
-      <c r="W41" t="n">
-        <v>0</v>
-      </c>
+      <c r="W41" t="inlineStr"/>
       <c r="X41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z41" t="n">
         <v>0</v>
@@ -4217,6 +4299,9 @@
         <v>0</v>
       </c>
       <c r="AC41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4290,13 +4375,13 @@
         <v>21218403</v>
       </c>
       <c r="W42" t="n">
-        <v>0</v>
+        <v>263</v>
       </c>
       <c r="X42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z42" t="n">
         <v>0</v>
@@ -4308,6 +4393,9 @@
         <v>0</v>
       </c>
       <c r="AC42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4380,14 +4468,12 @@
       <c r="V43" t="n">
         <v>12811858</v>
       </c>
-      <c r="W43" t="n">
-        <v>0</v>
-      </c>
+      <c r="W43" t="inlineStr"/>
       <c r="X43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z43" t="n">
         <v>0</v>
@@ -4399,6 +4485,9 @@
         <v>0</v>
       </c>
       <c r="AC43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4471,14 +4560,12 @@
       <c r="V44" t="n">
         <v>969869</v>
       </c>
-      <c r="W44" t="n">
-        <v>0</v>
-      </c>
+      <c r="W44" t="inlineStr"/>
       <c r="X44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z44" t="n">
         <v>0</v>
@@ -4490,6 +4577,9 @@
         <v>0</v>
       </c>
       <c r="AC44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4563,13 +4653,13 @@
         <v>1087585</v>
       </c>
       <c r="W45" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="X45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z45" t="n">
         <v>0</v>
@@ -4581,6 +4671,9 @@
         <v>0</v>
       </c>
       <c r="AC45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4654,10 +4747,10 @@
         <v>81903458</v>
       </c>
       <c r="W46" t="n">
-        <v>1</v>
+        <v>1644</v>
       </c>
       <c r="X46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y46" t="n">
         <v>0</v>
@@ -4672,6 +4765,9 @@
         <v>0</v>
       </c>
       <c r="AC46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4744,9 +4840,7 @@
       <c r="V47" t="n">
         <v>36850101</v>
       </c>
-      <c r="W47" t="n">
-        <v>0</v>
-      </c>
+      <c r="W47" t="inlineStr"/>
       <c r="X47" t="n">
         <v>0</v>
       </c>
@@ -4754,15 +4848,18 @@
         <v>0</v>
       </c>
       <c r="Z47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB47" t="n">
         <v>0</v>
       </c>
       <c r="AC47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4835,9 +4932,7 @@
       <c r="V48" t="n">
         <v>24650296</v>
       </c>
-      <c r="W48" t="n">
-        <v>0</v>
-      </c>
+      <c r="W48" t="inlineStr"/>
       <c r="X48" t="n">
         <v>0</v>
       </c>
@@ -4848,12 +4943,15 @@
         <v>0</v>
       </c>
       <c r="AA48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4926,14 +5024,12 @@
       <c r="V49" t="n">
         <v>130444603</v>
       </c>
-      <c r="W49" t="n">
-        <v>0</v>
-      </c>
+      <c r="W49" t="inlineStr"/>
       <c r="X49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z49" t="n">
         <v>0</v>
@@ -4945,6 +5041,9 @@
         <v>0</v>
       </c>
       <c r="AC49" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5017,14 +5116,12 @@
       <c r="V50" t="n">
         <v>12423831</v>
       </c>
-      <c r="W50" t="n">
-        <v>0</v>
-      </c>
+      <c r="W50" t="inlineStr"/>
       <c r="X50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z50" t="n">
         <v>0</v>
@@ -5036,6 +5133,9 @@
         <v>0</v>
       </c>
       <c r="AC50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5109,10 +5209,10 @@
         <v>65075540</v>
       </c>
       <c r="W51" t="n">
-        <v>1</v>
+        <v>1176</v>
       </c>
       <c r="X51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y51" t="n">
         <v>0</v>
@@ -5127,6 +5227,9 @@
         <v>0</v>
       </c>
       <c r="AC51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5199,17 +5302,15 @@
       <c r="V52" t="n">
         <v>455317.5</v>
       </c>
-      <c r="W52" t="n">
-        <v>0</v>
-      </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="n">
         <v>0</v>
       </c>
       <c r="Y52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA52" t="n">
         <v>0</v>
@@ -5218,6 +5319,9 @@
         <v>0</v>
       </c>
       <c r="AC52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5290,9 +5394,7 @@
       <c r="V53" t="n">
         <v>110101975</v>
       </c>
-      <c r="W53" t="n">
-        <v>0</v>
-      </c>
+      <c r="W53" t="inlineStr"/>
       <c r="X53" t="n">
         <v>0</v>
       </c>
@@ -5300,15 +5402,18 @@
         <v>0</v>
       </c>
       <c r="Z53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB53" t="n">
         <v>0</v>
       </c>
       <c r="AC53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5381,14 +5486,12 @@
       <c r="V54" t="n">
         <v>20324096</v>
       </c>
-      <c r="W54" t="n">
-        <v>0</v>
-      </c>
+      <c r="W54" t="inlineStr"/>
       <c r="X54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z54" t="n">
         <v>0</v>
@@ -5400,6 +5503,9 @@
         <v>0</v>
       </c>
       <c r="AC54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5473,10 +5579,10 @@
         <v>56629811.40740741</v>
       </c>
       <c r="W55" t="n">
-        <v>1</v>
+        <v>319</v>
       </c>
       <c r="X55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y55" t="n">
         <v>0</v>
@@ -5491,6 +5597,9 @@
         <v>0</v>
       </c>
       <c r="AC55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5564,13 +5673,13 @@
         <v>24065925.59677419</v>
       </c>
       <c r="W56" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="X56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z56" t="n">
         <v>0</v>
@@ -5582,6 +5691,9 @@
         <v>0</v>
       </c>
       <c r="AC56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5655,10 +5767,10 @@
         <v>83301580</v>
       </c>
       <c r="W57" t="n">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="X57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y57" t="n">
         <v>0</v>
@@ -5673,6 +5785,9 @@
         <v>0</v>
       </c>
       <c r="AC57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5745,14 +5860,12 @@
       <c r="V58" t="n">
         <v>3581642</v>
       </c>
-      <c r="W58" t="n">
-        <v>0</v>
-      </c>
+      <c r="W58" t="inlineStr"/>
       <c r="X58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z58" t="n">
         <v>0</v>
@@ -5764,6 +5877,9 @@
         <v>0</v>
       </c>
       <c r="AC58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5837,10 +5953,10 @@
         <v>10763520</v>
       </c>
       <c r="W59" t="n">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="X59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y59" t="n">
         <v>0</v>
@@ -5855,6 +5971,9 @@
         <v>0</v>
       </c>
       <c r="AC59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5928,16 +6047,16 @@
         <v>38493</v>
       </c>
       <c r="W60" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="X60" t="n">
         <v>0</v>
       </c>
       <c r="Y60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA60" t="n">
         <v>0</v>
@@ -5946,6 +6065,9 @@
         <v>0</v>
       </c>
       <c r="AC60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD60" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6019,7 +6141,7 @@
         <v>35291068</v>
       </c>
       <c r="W61" t="n">
-        <v>0</v>
+        <v>1063</v>
       </c>
       <c r="X61" t="n">
         <v>0</v>
@@ -6028,15 +6150,18 @@
         <v>0</v>
       </c>
       <c r="Z61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB61" t="n">
         <v>0</v>
       </c>
       <c r="AC61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6110,10 +6235,10 @@
         <v>63686397</v>
       </c>
       <c r="W62" t="n">
-        <v>1</v>
+        <v>2812</v>
       </c>
       <c r="X62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y62" t="n">
         <v>0</v>
@@ -6128,6 +6253,9 @@
         <v>0</v>
       </c>
       <c r="AC62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6201,10 +6329,10 @@
         <v>85364450</v>
       </c>
       <c r="W63" t="n">
-        <v>1</v>
+        <v>1195</v>
       </c>
       <c r="X63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y63" t="n">
         <v>0</v>
@@ -6219,6 +6347,9 @@
         <v>0</v>
       </c>
       <c r="AC63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6292,16 +6423,16 @@
         <v>455317.5</v>
       </c>
       <c r="W64" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="X64" t="n">
         <v>0</v>
       </c>
       <c r="Y64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA64" t="n">
         <v>0</v>
@@ -6310,6 +6441,9 @@
         <v>0</v>
       </c>
       <c r="AC64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6383,10 +6517,10 @@
         <v>45512466</v>
       </c>
       <c r="W65" t="n">
-        <v>1</v>
+        <v>935</v>
       </c>
       <c r="X65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y65" t="n">
         <v>0</v>
@@ -6401,6 +6535,9 @@
         <v>0</v>
       </c>
       <c r="AC65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6473,14 +6610,12 @@
       <c r="V66" t="n">
         <v>132399394</v>
       </c>
-      <c r="W66" t="n">
-        <v>0</v>
-      </c>
+      <c r="W66" t="inlineStr"/>
       <c r="X66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z66" t="n">
         <v>0</v>
@@ -6492,6 +6627,9 @@
         <v>0</v>
       </c>
       <c r="AC66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6565,13 +6703,13 @@
         <v>12134935</v>
       </c>
       <c r="W67" t="n">
-        <v>0</v>
+        <v>607</v>
       </c>
       <c r="X67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z67" t="n">
         <v>0</v>
@@ -6583,6 +6721,9 @@
         <v>0</v>
       </c>
       <c r="AC67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD67" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6656,13 +6797,13 @@
         <v>17300439</v>
       </c>
       <c r="W68" t="n">
-        <v>0</v>
+        <v>643</v>
       </c>
       <c r="X68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z68" t="n">
         <v>0</v>
@@ -6674,6 +6815,9 @@
         <v>0</v>
       </c>
       <c r="AC68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6747,10 +6891,10 @@
         <v>35857181</v>
       </c>
       <c r="W69" t="n">
-        <v>1</v>
+        <v>4022</v>
       </c>
       <c r="X69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y69" t="n">
         <v>0</v>
@@ -6765,6 +6909,9 @@
         <v>0</v>
       </c>
       <c r="AC69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6838,10 +6985,10 @@
         <v>26302731</v>
       </c>
       <c r="W70" t="n">
-        <v>1</v>
+        <v>508</v>
       </c>
       <c r="X70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y70" t="n">
         <v>0</v>
@@ -6856,6 +7003,9 @@
         <v>0</v>
       </c>
       <c r="AC70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6929,10 +7079,10 @@
         <v>15472775</v>
       </c>
       <c r="W71" t="n">
-        <v>1</v>
+        <v>1502</v>
       </c>
       <c r="X71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y71" t="n">
         <v>0</v>
@@ -6947,6 +7097,9 @@
         <v>0</v>
       </c>
       <c r="AC71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7020,10 +7173,10 @@
         <v>13303319</v>
       </c>
       <c r="W72" t="n">
-        <v>1</v>
+        <v>611</v>
       </c>
       <c r="X72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y72" t="n">
         <v>0</v>
@@ -7038,6 +7191,9 @@
         <v>0</v>
       </c>
       <c r="AC72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7110,9 +7266,7 @@
       <c r="V73" t="n">
         <v>52767889</v>
       </c>
-      <c r="W73" t="n">
-        <v>0</v>
-      </c>
+      <c r="W73" t="inlineStr"/>
       <c r="X73" t="n">
         <v>0</v>
       </c>
@@ -7120,15 +7274,18 @@
         <v>0</v>
       </c>
       <c r="Z73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB73" t="n">
         <v>0</v>
       </c>
       <c r="AC73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7205,10 +7362,10 @@
         <v>0</v>
       </c>
       <c r="X74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z74" t="n">
         <v>0</v>
@@ -7220,6 +7377,9 @@
         <v>0</v>
       </c>
       <c r="AC74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7296,10 +7456,10 @@
         <v>0</v>
       </c>
       <c r="X75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z75" t="n">
         <v>0</v>
@@ -7311,6 +7471,9 @@
         <v>0</v>
       </c>
       <c r="AC75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7383,14 +7546,12 @@
       <c r="V76" t="n">
         <v>11603545</v>
       </c>
-      <c r="W76" t="n">
-        <v>0</v>
-      </c>
+      <c r="W76" t="inlineStr"/>
       <c r="X76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z76" t="n">
         <v>0</v>
@@ -7402,6 +7563,9 @@
         <v>0</v>
       </c>
       <c r="AC76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7475,10 +7639,10 @@
         <v>44806783</v>
       </c>
       <c r="W77" t="n">
-        <v>1</v>
+        <v>606</v>
       </c>
       <c r="X77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y77" t="n">
         <v>0</v>
@@ -7493,6 +7657,9 @@
         <v>0</v>
       </c>
       <c r="AC77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7566,7 +7733,7 @@
         <v>62950384</v>
       </c>
       <c r="W78" t="n">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="X78" t="n">
         <v>0</v>
@@ -7575,15 +7742,18 @@
         <v>0</v>
       </c>
       <c r="Z78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB78" t="n">
         <v>0</v>
       </c>
       <c r="AC78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7657,13 +7827,13 @@
         <v>24065925.59677419</v>
       </c>
       <c r="W79" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="X79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z79" t="n">
         <v>0</v>
@@ -7675,6 +7845,9 @@
         <v>0</v>
       </c>
       <c r="AC79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7748,10 +7921,10 @@
         <v>101196</v>
       </c>
       <c r="W80" t="n">
-        <v>1</v>
+        <v>2356</v>
       </c>
       <c r="X80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y80" t="n">
         <v>0</v>
@@ -7766,6 +7939,9 @@
         <v>0</v>
       </c>
       <c r="AC80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7838,14 +8014,12 @@
       <c r="V81" t="n">
         <v>12482775</v>
       </c>
-      <c r="W81" t="n">
-        <v>0</v>
-      </c>
+      <c r="W81" t="inlineStr"/>
       <c r="X81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z81" t="n">
         <v>0</v>
@@ -7857,6 +8031,9 @@
         <v>0</v>
       </c>
       <c r="AC81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7929,11 +8106,9 @@
       <c r="V82" t="n">
         <v>213307889</v>
       </c>
-      <c r="W82" t="n">
-        <v>1</v>
-      </c>
+      <c r="W82" t="inlineStr"/>
       <c r="X82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y82" t="n">
         <v>0</v>
@@ -7948,6 +8123,9 @@
         <v>0</v>
       </c>
       <c r="AC82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8020,11 +8198,9 @@
       <c r="V83" t="n">
         <v>25785603</v>
       </c>
-      <c r="W83" t="n">
-        <v>1</v>
-      </c>
+      <c r="W83" t="inlineStr"/>
       <c r="X83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y83" t="n">
         <v>0</v>
@@ -8039,6 +8215,9 @@
         <v>0</v>
       </c>
       <c r="AC83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8111,14 +8290,12 @@
       <c r="V84" t="n">
         <v>30610863</v>
       </c>
-      <c r="W84" t="n">
-        <v>0</v>
-      </c>
+      <c r="W84" t="inlineStr"/>
       <c r="X84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z84" t="n">
         <v>0</v>
@@ -8130,6 +8307,9 @@
         <v>0</v>
       </c>
       <c r="AC84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8202,14 +8382,12 @@
       <c r="V85" t="n">
         <v>128505958</v>
       </c>
-      <c r="W85" t="n">
-        <v>0</v>
-      </c>
+      <c r="W85" t="inlineStr"/>
       <c r="X85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z85" t="n">
         <v>0</v>
@@ -8221,6 +8399,9 @@
         <v>0</v>
       </c>
       <c r="AC85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8294,13 +8475,13 @@
         <v>24065925.59677419</v>
       </c>
       <c r="W86" t="n">
-        <v>0</v>
+        <v>2635</v>
       </c>
       <c r="X86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z86" t="n">
         <v>0</v>
@@ -8312,6 +8493,9 @@
         <v>0</v>
       </c>
       <c r="AC86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8384,14 +8568,12 @@
       <c r="V87" t="n">
         <v>1132112</v>
       </c>
-      <c r="W87" t="n">
-        <v>0</v>
-      </c>
+      <c r="W87" t="inlineStr"/>
       <c r="X87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z87" t="n">
         <v>0</v>
@@ -8403,6 +8585,9 @@
         <v>0</v>
       </c>
       <c r="AC87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8476,13 +8661,13 @@
         <v>4211129</v>
       </c>
       <c r="W88" t="n">
-        <v>0</v>
+        <v>491</v>
       </c>
       <c r="X88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z88" t="n">
         <v>0</v>
@@ -8494,6 +8679,9 @@
         <v>0</v>
       </c>
       <c r="AC88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD88" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8567,13 +8755,13 @@
         <v>70958</v>
       </c>
       <c r="W89" t="n">
-        <v>0</v>
+        <v>1023</v>
       </c>
       <c r="X89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z89" t="n">
         <v>0</v>
@@ -8585,6 +8773,9 @@
         <v>0</v>
       </c>
       <c r="AC89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD89" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8657,14 +8848,12 @@
       <c r="V90" t="n">
         <v>591366</v>
       </c>
-      <c r="W90" t="n">
-        <v>0</v>
-      </c>
+      <c r="W90" t="inlineStr"/>
       <c r="X90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z90" t="n">
         <v>0</v>
@@ -8676,6 +8865,9 @@
         <v>0</v>
       </c>
       <c r="AC90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8748,11 +8940,9 @@
       <c r="V91" t="n">
         <v>20763013</v>
       </c>
-      <c r="W91" t="n">
-        <v>1</v>
-      </c>
+      <c r="W91" t="inlineStr"/>
       <c r="X91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y91" t="n">
         <v>0</v>
@@ -8767,6 +8957,9 @@
         <v>0</v>
       </c>
       <c r="AC91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD91" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8840,13 +9033,13 @@
         <v>24065925.59677419</v>
       </c>
       <c r="W92" t="n">
-        <v>0</v>
+        <v>469</v>
       </c>
       <c r="X92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z92" t="n">
         <v>0</v>
@@ -8858,6 +9051,9 @@
         <v>0</v>
       </c>
       <c r="AC92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8930,14 +9126,12 @@
       <c r="V93" t="n">
         <v>50000000</v>
       </c>
-      <c r="W93" t="n">
-        <v>0</v>
-      </c>
+      <c r="W93" t="inlineStr"/>
       <c r="X93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z93" t="n">
         <v>0</v>
@@ -8949,6 +9143,9 @@
         <v>0</v>
       </c>
       <c r="AC93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD93" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9022,7 +9219,7 @@
         <v>3909002</v>
       </c>
       <c r="W94" t="n">
-        <v>0</v>
+        <v>2283</v>
       </c>
       <c r="X94" t="n">
         <v>0</v>
@@ -9037,9 +9234,12 @@
         <v>0</v>
       </c>
       <c r="AB94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC94" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD94" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9112,9 +9312,7 @@
       <c r="V95" t="n">
         <v>160861908</v>
       </c>
-      <c r="W95" t="n">
-        <v>0</v>
-      </c>
+      <c r="W95" t="inlineStr"/>
       <c r="X95" t="n">
         <v>0</v>
       </c>
@@ -9122,15 +9320,18 @@
         <v>0</v>
       </c>
       <c r="Z95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB95" t="n">
         <v>0</v>
       </c>
       <c r="AC95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD95" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9203,14 +9404,12 @@
       <c r="V96" t="n">
         <v>54766923</v>
       </c>
-      <c r="W96" t="n">
-        <v>0</v>
-      </c>
+      <c r="W96" t="inlineStr"/>
       <c r="X96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z96" t="n">
         <v>0</v>
@@ -9222,6 +9421,9 @@
         <v>0</v>
       </c>
       <c r="AC96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD96" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9294,9 +9496,7 @@
       <c r="V97" t="n">
         <v>261441092</v>
       </c>
-      <c r="W97" t="n">
-        <v>0</v>
-      </c>
+      <c r="W97" t="inlineStr"/>
       <c r="X97" t="n">
         <v>0</v>
       </c>
@@ -9304,15 +9504,18 @@
         <v>0</v>
       </c>
       <c r="Z97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB97" t="n">
         <v>0</v>
       </c>
       <c r="AC97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD97" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9389,7 +9592,7 @@
         <v>1</v>
       </c>
       <c r="X98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y98" t="n">
         <v>0</v>
@@ -9404,6 +9607,9 @@
         <v>0</v>
       </c>
       <c r="AC98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9476,9 +9682,7 @@
       <c r="V99" t="n">
         <v>243640120</v>
       </c>
-      <c r="W99" t="n">
-        <v>0</v>
-      </c>
+      <c r="W99" t="inlineStr"/>
       <c r="X99" t="n">
         <v>0</v>
       </c>
@@ -9486,15 +9690,18 @@
         <v>0</v>
       </c>
       <c r="Z99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB99" t="n">
         <v>0</v>
       </c>
       <c r="AC99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD99" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9567,14 +9774,12 @@
       <c r="V100" t="n">
         <v>46236000</v>
       </c>
-      <c r="W100" t="n">
-        <v>0</v>
-      </c>
+      <c r="W100" t="inlineStr"/>
       <c r="X100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z100" t="n">
         <v>0</v>
@@ -9586,6 +9791,9 @@
         <v>0</v>
       </c>
       <c r="AC100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD100" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9659,7 +9867,7 @@
         <v>58715510</v>
       </c>
       <c r="W101" t="n">
-        <v>0</v>
+        <v>1011</v>
       </c>
       <c r="X101" t="n">
         <v>0</v>
@@ -9668,15 +9876,18 @@
         <v>0</v>
       </c>
       <c r="Z101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB101" t="n">
         <v>0</v>
       </c>
       <c r="AC101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD101" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9750,10 +9961,10 @@
         <v>30212620</v>
       </c>
       <c r="W102" t="n">
-        <v>1</v>
+        <v>1644</v>
       </c>
       <c r="X102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y102" t="n">
         <v>0</v>
@@ -9768,6 +9979,9 @@
         <v>0</v>
       </c>
       <c r="AC102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD102" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9840,14 +10054,12 @@
       <c r="V103" t="n">
         <v>560069</v>
       </c>
-      <c r="W103" t="n">
-        <v>0</v>
-      </c>
+      <c r="W103" t="inlineStr"/>
       <c r="X103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z103" t="n">
         <v>0</v>
@@ -9859,6 +10071,9 @@
         <v>0</v>
       </c>
       <c r="AC103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD103" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9931,9 +10146,7 @@
       <c r="V104" t="n">
         <v>155019340</v>
       </c>
-      <c r="W104" t="n">
-        <v>0</v>
-      </c>
+      <c r="W104" t="inlineStr"/>
       <c r="X104" t="n">
         <v>0</v>
       </c>
@@ -9941,15 +10154,18 @@
         <v>0</v>
       </c>
       <c r="Z104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB104" t="n">
         <v>0</v>
       </c>
       <c r="AC104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD104" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10023,10 +10239,10 @@
         <v>49438370</v>
       </c>
       <c r="W105" t="n">
-        <v>1</v>
+        <v>983</v>
       </c>
       <c r="X105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y105" t="n">
         <v>0</v>
@@ -10041,6 +10257,9 @@
         <v>0</v>
       </c>
       <c r="AC105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD105" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10113,9 +10332,7 @@
       <c r="V106" t="n">
         <v>61123569</v>
       </c>
-      <c r="W106" t="n">
-        <v>0</v>
-      </c>
+      <c r="W106" t="inlineStr"/>
       <c r="X106" t="n">
         <v>0</v>
       </c>
@@ -10123,15 +10340,18 @@
         <v>0</v>
       </c>
       <c r="Z106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB106" t="n">
         <v>0</v>
       </c>
       <c r="AC106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD106" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10205,10 +10425,10 @@
         <v>93953653</v>
       </c>
       <c r="W107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y107" t="n">
         <v>0</v>
@@ -10223,6 +10443,9 @@
         <v>0</v>
       </c>
       <c r="AC107" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD107" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10295,11 +10518,9 @@
       <c r="V108" t="n">
         <v>140125968</v>
       </c>
-      <c r="W108" t="n">
-        <v>1</v>
-      </c>
+      <c r="W108" t="inlineStr"/>
       <c r="X108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y108" t="n">
         <v>0</v>
@@ -10314,6 +10535,9 @@
         <v>0</v>
       </c>
       <c r="AC108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD108" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10387,13 +10611,13 @@
         <v>3242457</v>
       </c>
       <c r="W109" t="n">
-        <v>0</v>
+        <v>1094</v>
       </c>
       <c r="X109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z109" t="n">
         <v>0</v>
@@ -10405,6 +10629,9 @@
         <v>0</v>
       </c>
       <c r="AC109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD109" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10477,9 +10704,7 @@
       <c r="V110" t="n">
         <v>245852179</v>
       </c>
-      <c r="W110" t="n">
-        <v>0</v>
-      </c>
+      <c r="W110" t="inlineStr"/>
       <c r="X110" t="n">
         <v>0</v>
       </c>
@@ -10490,12 +10715,15 @@
         <v>0</v>
       </c>
       <c r="AA110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC110" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD110" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10568,14 +10796,12 @@
       <c r="V111" t="n">
         <v>42313354</v>
       </c>
-      <c r="W111" t="n">
-        <v>0</v>
-      </c>
+      <c r="W111" t="inlineStr"/>
       <c r="X111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z111" t="n">
         <v>0</v>
@@ -10587,6 +10813,9 @@
         <v>0</v>
       </c>
       <c r="AC111" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD111" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10659,14 +10888,12 @@
       <c r="V112" t="n">
         <v>3263585</v>
       </c>
-      <c r="W112" t="n">
-        <v>0</v>
-      </c>
+      <c r="W112" t="inlineStr"/>
       <c r="X112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z112" t="n">
         <v>0</v>
@@ -10678,6 +10905,9 @@
         <v>0</v>
       </c>
       <c r="AC112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD112" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10751,13 +10981,13 @@
         <v>18119640</v>
       </c>
       <c r="W113" t="n">
-        <v>0</v>
+        <v>478</v>
       </c>
       <c r="X113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z113" t="n">
         <v>0</v>
@@ -10769,6 +10999,9 @@
         <v>0</v>
       </c>
       <c r="AC113" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD113" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10841,11 +11074,9 @@
       <c r="V114" t="n">
         <v>55474756</v>
       </c>
-      <c r="W114" t="n">
-        <v>1</v>
-      </c>
+      <c r="W114" t="inlineStr"/>
       <c r="X114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y114" t="n">
         <v>0</v>
@@ -10860,6 +11091,9 @@
         <v>0</v>
       </c>
       <c r="AC114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD114" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10933,13 +11167,13 @@
         <v>14915773</v>
       </c>
       <c r="W115" t="n">
-        <v>0</v>
+        <v>362</v>
       </c>
       <c r="X115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z115" t="n">
         <v>0</v>
@@ -10951,6 +11185,9 @@
         <v>0</v>
       </c>
       <c r="AC115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD115" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11023,9 +11260,7 @@
       <c r="V116" t="n">
         <v>102247150</v>
       </c>
-      <c r="W116" t="n">
-        <v>0</v>
-      </c>
+      <c r="W116" t="inlineStr"/>
       <c r="X116" t="n">
         <v>0</v>
       </c>
@@ -11042,6 +11277,9 @@
         <v>0</v>
       </c>
       <c r="AC116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD116" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11114,11 +11352,9 @@
       <c r="V117" t="n">
         <v>70136369</v>
       </c>
-      <c r="W117" t="n">
-        <v>1</v>
-      </c>
+      <c r="W117" t="inlineStr"/>
       <c r="X117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y117" t="n">
         <v>0</v>
@@ -11133,6 +11369,9 @@
         <v>0</v>
       </c>
       <c r="AC117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD117" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11205,9 +11444,7 @@
       <c r="V118" t="n">
         <v>60106536</v>
       </c>
-      <c r="W118" t="n">
-        <v>0</v>
-      </c>
+      <c r="W118" t="inlineStr"/>
       <c r="X118" t="n">
         <v>0</v>
       </c>
@@ -11215,15 +11452,18 @@
         <v>0</v>
       </c>
       <c r="Z118" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB118" t="n">
         <v>0</v>
       </c>
       <c r="AC118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD118" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11296,11 +11536,9 @@
       <c r="V119" t="n">
         <v>13167232</v>
       </c>
-      <c r="W119" t="n">
-        <v>1</v>
-      </c>
+      <c r="W119" t="inlineStr"/>
       <c r="X119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y119" t="n">
         <v>0</v>
@@ -11315,6 +11553,9 @@
         <v>0</v>
       </c>
       <c r="AC119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD119" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11387,14 +11628,12 @@
       <c r="V120" t="n">
         <v>2832029</v>
       </c>
-      <c r="W120" t="n">
-        <v>0</v>
-      </c>
+      <c r="W120" t="inlineStr"/>
       <c r="X120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z120" t="n">
         <v>0</v>
@@ -11406,6 +11645,9 @@
         <v>0</v>
       </c>
       <c r="AC120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD120" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11479,13 +11721,13 @@
         <v>316472</v>
       </c>
       <c r="W121" t="n">
-        <v>0</v>
+        <v>731</v>
       </c>
       <c r="X121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z121" t="n">
         <v>0</v>
@@ -11497,6 +11739,9 @@
         <v>0</v>
       </c>
       <c r="AC121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD121" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11569,14 +11814,12 @@
       <c r="V122" t="n">
         <v>33479698</v>
       </c>
-      <c r="W122" t="n">
-        <v>0</v>
-      </c>
+      <c r="W122" t="inlineStr"/>
       <c r="X122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z122" t="n">
         <v>0</v>
@@ -11588,6 +11831,9 @@
         <v>0</v>
       </c>
       <c r="AC122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD122" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11660,9 +11906,7 @@
       <c r="V123" t="n">
         <v>7266383</v>
       </c>
-      <c r="W123" t="n">
-        <v>0</v>
-      </c>
+      <c r="W123" t="inlineStr"/>
       <c r="X123" t="n">
         <v>0</v>
       </c>
@@ -11670,15 +11914,18 @@
         <v>0</v>
       </c>
       <c r="Z123" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB123" t="n">
         <v>0</v>
       </c>
       <c r="AC123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD123" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11751,14 +11998,12 @@
       <c r="V124" t="n">
         <v>236452</v>
       </c>
-      <c r="W124" t="n">
-        <v>0</v>
-      </c>
+      <c r="W124" t="inlineStr"/>
       <c r="X124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z124" t="n">
         <v>0</v>
@@ -11770,6 +12015,9 @@
         <v>0</v>
       </c>
       <c r="AC124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD124" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11842,14 +12090,12 @@
       <c r="V125" t="n">
         <v>67436818</v>
       </c>
-      <c r="W125" t="n">
-        <v>0</v>
-      </c>
+      <c r="W125" t="inlineStr"/>
       <c r="X125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z125" t="n">
         <v>0</v>
@@ -11861,6 +12107,9 @@
         <v>0</v>
       </c>
       <c r="AC125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD125" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11933,14 +12182,12 @@
       <c r="V126" t="n">
         <v>2201923</v>
       </c>
-      <c r="W126" t="n">
-        <v>0</v>
-      </c>
+      <c r="W126" t="inlineStr"/>
       <c r="X126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z126" t="n">
         <v>0</v>
@@ -11952,6 +12199,9 @@
         <v>0</v>
       </c>
       <c r="AC126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD126" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12025,16 +12275,16 @@
         <v>455317.5</v>
       </c>
       <c r="W127" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X127" t="n">
         <v>0</v>
       </c>
       <c r="Y127" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA127" t="n">
         <v>0</v>
@@ -12043,6 +12293,9 @@
         <v>0</v>
       </c>
       <c r="AC127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD127" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12115,14 +12368,12 @@
       <c r="V128" t="n">
         <v>7434726</v>
       </c>
-      <c r="W128" t="n">
-        <v>0</v>
-      </c>
+      <c r="W128" t="inlineStr"/>
       <c r="X128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z128" t="n">
         <v>0</v>
@@ -12134,6 +12385,9 @@
         <v>0</v>
       </c>
       <c r="AC128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD128" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12206,14 +12460,12 @@
       <c r="V129" t="n">
         <v>2678691</v>
       </c>
-      <c r="W129" t="n">
-        <v>0</v>
-      </c>
+      <c r="W129" t="inlineStr"/>
       <c r="X129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z129" t="n">
         <v>0</v>
@@ -12225,6 +12477,9 @@
         <v>0</v>
       </c>
       <c r="AC129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD129" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12297,9 +12552,7 @@
       <c r="V130" t="n">
         <v>17323326</v>
       </c>
-      <c r="W130" t="n">
-        <v>0</v>
-      </c>
+      <c r="W130" t="inlineStr"/>
       <c r="X130" t="n">
         <v>0</v>
       </c>
@@ -12307,15 +12560,18 @@
         <v>0</v>
       </c>
       <c r="Z130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB130" t="n">
         <v>0</v>
       </c>
       <c r="AC130" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD130" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12389,10 +12645,10 @@
         <v>1730597</v>
       </c>
       <c r="W131" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="X131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y131" t="n">
         <v>0</v>
@@ -12407,6 +12663,9 @@
         <v>0</v>
       </c>
       <c r="AC131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD131" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12479,9 +12738,7 @@
       <c r="V132" t="n">
         <v>219964115</v>
       </c>
-      <c r="W132" t="n">
-        <v>0</v>
-      </c>
+      <c r="W132" t="inlineStr"/>
       <c r="X132" t="n">
         <v>0</v>
       </c>
@@ -12489,15 +12746,18 @@
         <v>0</v>
       </c>
       <c r="Z132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB132" t="n">
         <v>0</v>
       </c>
       <c r="AC132" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD132" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12570,14 +12830,12 @@
       <c r="V133" t="n">
         <v>14377198</v>
       </c>
-      <c r="W133" t="n">
-        <v>0</v>
-      </c>
+      <c r="W133" t="inlineStr"/>
       <c r="X133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z133" t="n">
         <v>0</v>
@@ -12589,6 +12847,9 @@
         <v>0</v>
       </c>
       <c r="AC133" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD133" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12660,16 +12921,16 @@
       </c>
       <c r="V134" t="inlineStr"/>
       <c r="W134" t="n">
-        <v>0</v>
+        <v>3153</v>
       </c>
       <c r="X134" t="n">
         <v>0</v>
       </c>
       <c r="Y134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA134" t="n">
         <v>0</v>
@@ -12678,6 +12939,9 @@
         <v>0</v>
       </c>
       <c r="AC134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD134" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Year in hot_encodings_df
</commit_message>
<xml_diff>
--- a/data/formatted/movies_one_hot_encodings.xlsx
+++ b/data/formatted/movies_one_hot_encodings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD134"/>
+  <dimension ref="A1:AE134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,35 +551,40 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
           <t>PG-13</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Unrated</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>PG</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>NC-17</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Approved</t>
         </is>
@@ -658,10 +663,10 @@
         <v>1068</v>
       </c>
       <c r="X2" t="n">
-        <v>1</v>
+        <v>2015</v>
       </c>
       <c r="Y2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2" t="n">
         <v>0</v>
@@ -676,6 +681,9 @@
         <v>0</v>
       </c>
       <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -750,13 +758,13 @@
       </c>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>1974</v>
       </c>
       <c r="Y3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" t="n">
         <v>0</v>
@@ -768,6 +776,9 @@
         <v>0</v>
       </c>
       <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -842,13 +853,13 @@
       </c>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>2005</v>
       </c>
       <c r="Y4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" t="n">
         <v>0</v>
@@ -860,6 +871,9 @@
         <v>0</v>
       </c>
       <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -934,13 +948,13 @@
       </c>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>2004</v>
       </c>
       <c r="Y5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5" t="n">
         <v>0</v>
@@ -952,6 +966,9 @@
         <v>0</v>
       </c>
       <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1028,13 +1045,13 @@
         <v>60</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
+        <v>2011</v>
       </c>
       <c r="Y6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" t="n">
         <v>0</v>
@@ -1046,6 +1063,9 @@
         <v>0</v>
       </c>
       <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1120,16 +1140,16 @@
       </c>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="n">
-        <v>0</v>
+        <v>2002</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7" t="n">
         <v>0</v>
@@ -1138,6 +1158,9 @@
         <v>0</v>
       </c>
       <c r="AD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1214,13 +1237,13 @@
         <v>421</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>2017</v>
       </c>
       <c r="Y8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8" t="n">
         <v>0</v>
@@ -1232,6 +1255,9 @@
         <v>0</v>
       </c>
       <c r="AD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1308,13 +1334,13 @@
         <v>72</v>
       </c>
       <c r="X9" t="n">
-        <v>0</v>
+        <v>2013</v>
       </c>
       <c r="Y9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9" t="n">
         <v>0</v>
@@ -1326,6 +1352,9 @@
         <v>0</v>
       </c>
       <c r="AD9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1402,13 +1431,13 @@
         <v>2770</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>2015</v>
       </c>
       <c r="Y10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10" t="n">
         <v>0</v>
@@ -1420,6 +1449,9 @@
         <v>0</v>
       </c>
       <c r="AD10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1496,10 +1528,10 @@
         <v>333</v>
       </c>
       <c r="X11" t="n">
-        <v>1</v>
+        <v>2021</v>
       </c>
       <c r="Y11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="n">
         <v>0</v>
@@ -1514,6 +1546,9 @@
         <v>0</v>
       </c>
       <c r="AD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1590,13 +1625,13 @@
         <v>856</v>
       </c>
       <c r="X12" t="n">
-        <v>0</v>
+        <v>2016</v>
       </c>
       <c r="Y12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA12" t="n">
         <v>0</v>
@@ -1608,6 +1643,9 @@
         <v>0</v>
       </c>
       <c r="AD12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1684,13 +1722,13 @@
         <v>125</v>
       </c>
       <c r="X13" t="n">
-        <v>0</v>
+        <v>2016</v>
       </c>
       <c r="Y13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA13" t="n">
         <v>0</v>
@@ -1702,6 +1740,9 @@
         <v>0</v>
       </c>
       <c r="AD13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1776,13 +1817,13 @@
       </c>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="Y14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14" t="n">
         <v>0</v>
@@ -1794,6 +1835,9 @@
         <v>0</v>
       </c>
       <c r="AD14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1868,13 +1912,13 @@
       </c>
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="n">
-        <v>0</v>
+        <v>1986</v>
       </c>
       <c r="Y15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15" t="n">
         <v>0</v>
@@ -1886,6 +1930,9 @@
         <v>0</v>
       </c>
       <c r="AD15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1962,10 +2009,10 @@
         <v>638</v>
       </c>
       <c r="X16" t="n">
-        <v>1</v>
+        <v>2018</v>
       </c>
       <c r="Y16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z16" t="n">
         <v>0</v>
@@ -1980,6 +2027,9 @@
         <v>0</v>
       </c>
       <c r="AD16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2056,7 +2106,7 @@
         <v>153</v>
       </c>
       <c r="X17" t="n">
-        <v>0</v>
+        <v>2016</v>
       </c>
       <c r="Y17" t="n">
         <v>0</v>
@@ -2065,15 +2115,18 @@
         <v>0</v>
       </c>
       <c r="AA17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC17" t="n">
         <v>0</v>
       </c>
       <c r="AD17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2148,13 +2201,13 @@
       </c>
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="Y18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA18" t="n">
         <v>0</v>
@@ -2166,6 +2219,9 @@
         <v>0</v>
       </c>
       <c r="AD18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2240,16 +2296,16 @@
       </c>
       <c r="W19" t="inlineStr"/>
       <c r="X19" t="n">
-        <v>0</v>
+        <v>2005</v>
       </c>
       <c r="Y19" t="n">
         <v>0</v>
       </c>
       <c r="Z19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB19" t="n">
         <v>0</v>
@@ -2258,6 +2314,9 @@
         <v>0</v>
       </c>
       <c r="AD19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2334,13 +2393,13 @@
         <v>866</v>
       </c>
       <c r="X20" t="n">
-        <v>0</v>
+        <v>2015</v>
       </c>
       <c r="Y20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA20" t="n">
         <v>0</v>
@@ -2352,6 +2411,9 @@
         <v>0</v>
       </c>
       <c r="AD20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2426,7 +2488,7 @@
       </c>
       <c r="W21" t="inlineStr"/>
       <c r="X21" t="n">
-        <v>0</v>
+        <v>1975</v>
       </c>
       <c r="Y21" t="n">
         <v>0</v>
@@ -2435,15 +2497,18 @@
         <v>0</v>
       </c>
       <c r="AA21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21" t="n">
         <v>0</v>
       </c>
       <c r="AD21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2518,13 +2583,13 @@
       </c>
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="n">
-        <v>0</v>
+        <v>1991</v>
       </c>
       <c r="Y22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA22" t="n">
         <v>0</v>
@@ -2536,6 +2601,9 @@
         <v>0</v>
       </c>
       <c r="AD22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2612,13 +2680,13 @@
         <v>63</v>
       </c>
       <c r="X23" t="n">
-        <v>0</v>
+        <v>2009</v>
       </c>
       <c r="Y23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA23" t="n">
         <v>0</v>
@@ -2630,6 +2698,9 @@
         <v>0</v>
       </c>
       <c r="AD23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2704,13 +2775,13 @@
       </c>
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="n">
-        <v>0</v>
+        <v>2002</v>
       </c>
       <c r="Y24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA24" t="n">
         <v>0</v>
@@ -2722,6 +2793,9 @@
         <v>0</v>
       </c>
       <c r="AD24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2796,13 +2870,13 @@
       </c>
       <c r="W25" t="inlineStr"/>
       <c r="X25" t="n">
-        <v>0</v>
+        <v>2004</v>
       </c>
       <c r="Y25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA25" t="n">
         <v>0</v>
@@ -2814,6 +2888,9 @@
         <v>0</v>
       </c>
       <c r="AD25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2888,13 +2965,13 @@
       </c>
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="Y26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA26" t="n">
         <v>0</v>
@@ -2906,6 +2983,9 @@
         <v>0</v>
       </c>
       <c r="AD26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2980,13 +3060,13 @@
       </c>
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="n">
-        <v>0</v>
+        <v>2006</v>
       </c>
       <c r="Y27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA27" t="n">
         <v>0</v>
@@ -2998,6 +3078,9 @@
         <v>0</v>
       </c>
       <c r="AD27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3074,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="X28" t="n">
-        <v>0</v>
+        <v>2018</v>
       </c>
       <c r="Y28" t="n">
         <v>0</v>
@@ -3083,15 +3166,18 @@
         <v>0</v>
       </c>
       <c r="AA28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC28" t="n">
         <v>0</v>
       </c>
       <c r="AD28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3166,7 +3252,7 @@
       </c>
       <c r="W29" t="inlineStr"/>
       <c r="X29" t="n">
-        <v>0</v>
+        <v>1939</v>
       </c>
       <c r="Y29" t="n">
         <v>0</v>
@@ -3178,12 +3264,15 @@
         <v>0</v>
       </c>
       <c r="AB29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3258,10 +3347,10 @@
       </c>
       <c r="W30" t="inlineStr"/>
       <c r="X30" t="n">
-        <v>1</v>
+        <v>1996</v>
       </c>
       <c r="Y30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z30" t="n">
         <v>0</v>
@@ -3276,6 +3365,9 @@
         <v>0</v>
       </c>
       <c r="AD30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3352,13 +3444,13 @@
         <v>1025</v>
       </c>
       <c r="X31" t="n">
-        <v>0</v>
+        <v>2020</v>
       </c>
       <c r="Y31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA31" t="n">
         <v>0</v>
@@ -3370,6 +3462,9 @@
         <v>0</v>
       </c>
       <c r="AD31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3446,13 +3541,13 @@
         <v>198</v>
       </c>
       <c r="X32" t="n">
-        <v>0</v>
+        <v>2014</v>
       </c>
       <c r="Y32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA32" t="n">
         <v>0</v>
@@ -3464,6 +3559,9 @@
         <v>0</v>
       </c>
       <c r="AD32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3538,7 +3636,7 @@
       </c>
       <c r="W33" t="inlineStr"/>
       <c r="X33" t="n">
-        <v>0</v>
+        <v>1984</v>
       </c>
       <c r="Y33" t="n">
         <v>0</v>
@@ -3547,15 +3645,18 @@
         <v>0</v>
       </c>
       <c r="AA33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC33" t="n">
         <v>0</v>
       </c>
       <c r="AD33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3632,13 +3733,13 @@
         <v>4785</v>
       </c>
       <c r="X34" t="n">
-        <v>0</v>
+        <v>2017</v>
       </c>
       <c r="Y34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA34" t="n">
         <v>0</v>
@@ -3650,6 +3751,9 @@
         <v>0</v>
       </c>
       <c r="AD34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3726,16 +3830,16 @@
         <v>276</v>
       </c>
       <c r="X35" t="n">
-        <v>0</v>
+        <v>2015</v>
       </c>
       <c r="Y35" t="n">
         <v>0</v>
       </c>
       <c r="Z35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB35" t="n">
         <v>0</v>
@@ -3744,6 +3848,9 @@
         <v>0</v>
       </c>
       <c r="AD35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3818,13 +3925,13 @@
       </c>
       <c r="W36" t="inlineStr"/>
       <c r="X36" t="n">
-        <v>0</v>
+        <v>1997</v>
       </c>
       <c r="Y36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA36" t="n">
         <v>0</v>
@@ -3836,6 +3943,9 @@
         <v>0</v>
       </c>
       <c r="AD36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3910,13 +4020,13 @@
       </c>
       <c r="W37" t="inlineStr"/>
       <c r="X37" t="n">
-        <v>0</v>
+        <v>1986</v>
       </c>
       <c r="Y37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA37" t="n">
         <v>0</v>
@@ -3928,6 +4038,9 @@
         <v>0</v>
       </c>
       <c r="AD37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4004,13 +4117,13 @@
         <v>14</v>
       </c>
       <c r="X38" t="n">
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="Y38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA38" t="n">
         <v>0</v>
@@ -4022,6 +4135,9 @@
         <v>0</v>
       </c>
       <c r="AD38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4098,13 +4214,13 @@
         <v>628</v>
       </c>
       <c r="X39" t="n">
-        <v>0</v>
+        <v>2009</v>
       </c>
       <c r="Y39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA39" t="n">
         <v>0</v>
@@ -4116,6 +4232,9 @@
         <v>0</v>
       </c>
       <c r="AD39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4192,10 +4311,10 @@
         <v>259</v>
       </c>
       <c r="X40" t="n">
-        <v>1</v>
+        <v>2012</v>
       </c>
       <c r="Y40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z40" t="n">
         <v>0</v>
@@ -4210,6 +4329,9 @@
         <v>0</v>
       </c>
       <c r="AD40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4284,13 +4406,13 @@
       </c>
       <c r="W41" t="inlineStr"/>
       <c r="X41" t="n">
-        <v>0</v>
+        <v>1991</v>
       </c>
       <c r="Y41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA41" t="n">
         <v>0</v>
@@ -4302,6 +4424,9 @@
         <v>0</v>
       </c>
       <c r="AD41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4378,13 +4503,13 @@
         <v>263</v>
       </c>
       <c r="X42" t="n">
-        <v>0</v>
+        <v>2016</v>
       </c>
       <c r="Y42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA42" t="n">
         <v>0</v>
@@ -4396,6 +4521,9 @@
         <v>0</v>
       </c>
       <c r="AD42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4470,13 +4598,13 @@
       </c>
       <c r="W43" t="inlineStr"/>
       <c r="X43" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="Y43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA43" t="n">
         <v>0</v>
@@ -4488,6 +4616,9 @@
         <v>0</v>
       </c>
       <c r="AD43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4562,13 +4693,13 @@
       </c>
       <c r="W44" t="inlineStr"/>
       <c r="X44" t="n">
-        <v>0</v>
+        <v>2007</v>
       </c>
       <c r="Y44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA44" t="n">
         <v>0</v>
@@ -4580,6 +4711,9 @@
         <v>0</v>
       </c>
       <c r="AD44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4656,13 +4790,13 @@
         <v>28</v>
       </c>
       <c r="X45" t="n">
-        <v>0</v>
+        <v>2016</v>
       </c>
       <c r="Y45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA45" t="n">
         <v>0</v>
@@ -4674,6 +4808,9 @@
         <v>0</v>
       </c>
       <c r="AD45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4750,10 +4887,10 @@
         <v>1644</v>
       </c>
       <c r="X46" t="n">
-        <v>1</v>
+        <v>2017</v>
       </c>
       <c r="Y46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z46" t="n">
         <v>0</v>
@@ -4768,6 +4905,9 @@
         <v>0</v>
       </c>
       <c r="AD46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4842,7 +4982,7 @@
       </c>
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="n">
-        <v>0</v>
+        <v>1999</v>
       </c>
       <c r="Y47" t="n">
         <v>0</v>
@@ -4851,15 +4991,18 @@
         <v>0</v>
       </c>
       <c r="AA47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC47" t="n">
         <v>0</v>
       </c>
       <c r="AD47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4934,7 +5077,7 @@
       </c>
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="n">
-        <v>0</v>
+        <v>1992</v>
       </c>
       <c r="Y48" t="n">
         <v>0</v>
@@ -4946,12 +5089,15 @@
         <v>0</v>
       </c>
       <c r="AB48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5026,13 +5172,13 @@
       </c>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="n">
-        <v>0</v>
+        <v>1998</v>
       </c>
       <c r="Y49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA49" t="n">
         <v>0</v>
@@ -5044,6 +5190,9 @@
         <v>0</v>
       </c>
       <c r="AD49" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5118,13 +5267,13 @@
       </c>
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="n">
-        <v>0</v>
+        <v>1987</v>
       </c>
       <c r="Y50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA50" t="n">
         <v>0</v>
@@ -5136,6 +5285,9 @@
         <v>0</v>
       </c>
       <c r="AD50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5212,10 +5364,10 @@
         <v>1176</v>
       </c>
       <c r="X51" t="n">
-        <v>1</v>
+        <v>2016</v>
       </c>
       <c r="Y51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z51" t="n">
         <v>0</v>
@@ -5230,6 +5382,9 @@
         <v>0</v>
       </c>
       <c r="AD51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5304,16 +5459,16 @@
       </c>
       <c r="W52" t="inlineStr"/>
       <c r="X52" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="Y52" t="n">
         <v>0</v>
       </c>
       <c r="Z52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB52" t="n">
         <v>0</v>
@@ -5322,6 +5477,9 @@
         <v>0</v>
       </c>
       <c r="AD52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5396,7 +5554,7 @@
       </c>
       <c r="W53" t="inlineStr"/>
       <c r="X53" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="Y53" t="n">
         <v>0</v>
@@ -5405,15 +5563,18 @@
         <v>0</v>
       </c>
       <c r="AA53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC53" t="n">
         <v>0</v>
       </c>
       <c r="AD53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5488,13 +5649,13 @@
       </c>
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="n">
-        <v>0</v>
+        <v>1988</v>
       </c>
       <c r="Y54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA54" t="n">
         <v>0</v>
@@ -5506,6 +5667,9 @@
         <v>0</v>
       </c>
       <c r="AD54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5582,10 +5746,10 @@
         <v>319</v>
       </c>
       <c r="X55" t="n">
-        <v>1</v>
+        <v>2015</v>
       </c>
       <c r="Y55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z55" t="n">
         <v>0</v>
@@ -5600,6 +5764,9 @@
         <v>0</v>
       </c>
       <c r="AD55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5676,13 +5843,13 @@
         <v>50</v>
       </c>
       <c r="X56" t="n">
-        <v>0</v>
+        <v>2017</v>
       </c>
       <c r="Y56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA56" t="n">
         <v>0</v>
@@ -5694,6 +5861,9 @@
         <v>0</v>
       </c>
       <c r="AD56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5770,10 +5940,10 @@
         <v>350</v>
       </c>
       <c r="X57" t="n">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="Y57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z57" t="n">
         <v>0</v>
@@ -5788,6 +5958,9 @@
         <v>0</v>
       </c>
       <c r="AD57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5862,13 +6035,13 @@
       </c>
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="Y58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA58" t="n">
         <v>0</v>
@@ -5880,6 +6053,9 @@
         <v>0</v>
       </c>
       <c r="AD58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5956,10 +6132,10 @@
         <v>61</v>
       </c>
       <c r="X59" t="n">
-        <v>1</v>
+        <v>2018</v>
       </c>
       <c r="Y59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z59" t="n">
         <v>0</v>
@@ -5974,6 +6150,9 @@
         <v>0</v>
       </c>
       <c r="AD59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6050,16 +6229,16 @@
         <v>24</v>
       </c>
       <c r="X60" t="n">
-        <v>0</v>
+        <v>2012</v>
       </c>
       <c r="Y60" t="n">
         <v>0</v>
       </c>
       <c r="Z60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB60" t="n">
         <v>0</v>
@@ -6068,6 +6247,9 @@
         <v>0</v>
       </c>
       <c r="AD60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE60" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6144,7 +6326,7 @@
         <v>1063</v>
       </c>
       <c r="X61" t="n">
-        <v>0</v>
+        <v>2012</v>
       </c>
       <c r="Y61" t="n">
         <v>0</v>
@@ -6153,15 +6335,18 @@
         <v>0</v>
       </c>
       <c r="AA61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC61" t="n">
         <v>0</v>
       </c>
       <c r="AD61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6238,10 +6423,10 @@
         <v>2812</v>
       </c>
       <c r="X62" t="n">
-        <v>1</v>
+        <v>2011</v>
       </c>
       <c r="Y62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z62" t="n">
         <v>0</v>
@@ -6256,6 +6441,9 @@
         <v>0</v>
       </c>
       <c r="AD62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6332,10 +6520,10 @@
         <v>1195</v>
       </c>
       <c r="X63" t="n">
-        <v>1</v>
+        <v>2017</v>
       </c>
       <c r="Y63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z63" t="n">
         <v>0</v>
@@ -6350,6 +6538,9 @@
         <v>0</v>
       </c>
       <c r="AD63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6426,16 +6617,16 @@
         <v>19</v>
       </c>
       <c r="X64" t="n">
-        <v>0</v>
+        <v>2018</v>
       </c>
       <c r="Y64" t="n">
         <v>0</v>
       </c>
       <c r="Z64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB64" t="n">
         <v>0</v>
@@ -6444,6 +6635,9 @@
         <v>0</v>
       </c>
       <c r="AD64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6520,10 +6714,10 @@
         <v>935</v>
       </c>
       <c r="X65" t="n">
-        <v>1</v>
+        <v>2012</v>
       </c>
       <c r="Y65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z65" t="n">
         <v>0</v>
@@ -6538,6 +6732,9 @@
         <v>0</v>
       </c>
       <c r="AD65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6612,13 +6809,13 @@
       </c>
       <c r="W66" t="inlineStr"/>
       <c r="X66" t="n">
-        <v>0</v>
+        <v>2006</v>
       </c>
       <c r="Y66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA66" t="n">
         <v>0</v>
@@ -6630,6 +6827,9 @@
         <v>0</v>
       </c>
       <c r="AD66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6706,13 +6906,13 @@
         <v>607</v>
       </c>
       <c r="X67" t="n">
-        <v>0</v>
+        <v>2010</v>
       </c>
       <c r="Y67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA67" t="n">
         <v>0</v>
@@ -6724,6 +6924,9 @@
         <v>0</v>
       </c>
       <c r="AD67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE67" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6800,13 +7003,13 @@
         <v>643</v>
       </c>
       <c r="X68" t="n">
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="Y68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA68" t="n">
         <v>0</v>
@@ -6818,6 +7021,9 @@
         <v>0</v>
       </c>
       <c r="AD68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6894,10 +7100,10 @@
         <v>4022</v>
       </c>
       <c r="X69" t="n">
-        <v>1</v>
+        <v>2018</v>
       </c>
       <c r="Y69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z69" t="n">
         <v>0</v>
@@ -6912,6 +7118,9 @@
         <v>0</v>
       </c>
       <c r="AD69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6988,10 +7197,10 @@
         <v>508</v>
       </c>
       <c r="X70" t="n">
-        <v>1</v>
+        <v>2015</v>
       </c>
       <c r="Y70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z70" t="n">
         <v>0</v>
@@ -7006,6 +7215,9 @@
         <v>0</v>
       </c>
       <c r="AD70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7082,10 +7294,10 @@
         <v>1502</v>
       </c>
       <c r="X71" t="n">
-        <v>1</v>
+        <v>2020</v>
       </c>
       <c r="Y71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z71" t="n">
         <v>0</v>
@@ -7100,6 +7312,9 @@
         <v>0</v>
       </c>
       <c r="AD71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7176,10 +7391,10 @@
         <v>611</v>
       </c>
       <c r="X72" t="n">
-        <v>1</v>
+        <v>2011</v>
       </c>
       <c r="Y72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z72" t="n">
         <v>0</v>
@@ -7194,6 +7409,9 @@
         <v>0</v>
       </c>
       <c r="AD72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7268,7 +7486,7 @@
       </c>
       <c r="W73" t="inlineStr"/>
       <c r="X73" t="n">
-        <v>0</v>
+        <v>1982</v>
       </c>
       <c r="Y73" t="n">
         <v>0</v>
@@ -7277,15 +7495,18 @@
         <v>0</v>
       </c>
       <c r="AA73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC73" t="n">
         <v>0</v>
       </c>
       <c r="AD73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7362,13 +7583,13 @@
         <v>0</v>
       </c>
       <c r="X74" t="n">
-        <v>0</v>
+        <v>2009</v>
       </c>
       <c r="Y74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA74" t="n">
         <v>0</v>
@@ -7380,6 +7601,9 @@
         <v>0</v>
       </c>
       <c r="AD74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7456,13 +7680,13 @@
         <v>0</v>
       </c>
       <c r="X75" t="n">
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="Y75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA75" t="n">
         <v>0</v>
@@ -7474,6 +7698,9 @@
         <v>0</v>
       </c>
       <c r="AD75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7548,13 +7775,13 @@
       </c>
       <c r="W76" t="inlineStr"/>
       <c r="X76" t="n">
-        <v>0</v>
+        <v>1985</v>
       </c>
       <c r="Y76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA76" t="n">
         <v>0</v>
@@ -7566,6 +7793,9 @@
         <v>0</v>
       </c>
       <c r="AD76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7642,10 +7872,10 @@
         <v>606</v>
       </c>
       <c r="X77" t="n">
-        <v>1</v>
+        <v>2012</v>
       </c>
       <c r="Y77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z77" t="n">
         <v>0</v>
@@ -7660,6 +7890,9 @@
         <v>0</v>
       </c>
       <c r="AD77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7736,7 +7969,7 @@
         <v>1469</v>
       </c>
       <c r="X78" t="n">
-        <v>0</v>
+        <v>2010</v>
       </c>
       <c r="Y78" t="n">
         <v>0</v>
@@ -7745,15 +7978,18 @@
         <v>0</v>
       </c>
       <c r="AA78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC78" t="n">
         <v>0</v>
       </c>
       <c r="AD78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7830,13 +8066,13 @@
         <v>85</v>
       </c>
       <c r="X79" t="n">
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="Y79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA79" t="n">
         <v>0</v>
@@ -7848,6 +8084,9 @@
         <v>0</v>
       </c>
       <c r="AD79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7924,10 +8163,10 @@
         <v>2356</v>
       </c>
       <c r="X80" t="n">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="Y80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z80" t="n">
         <v>0</v>
@@ -7942,6 +8181,9 @@
         <v>0</v>
       </c>
       <c r="AD80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8016,13 +8258,13 @@
       </c>
       <c r="W81" t="inlineStr"/>
       <c r="X81" t="n">
-        <v>0</v>
+        <v>2005</v>
       </c>
       <c r="Y81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA81" t="n">
         <v>0</v>
@@ -8034,6 +8276,9 @@
         <v>0</v>
       </c>
       <c r="AD81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8108,10 +8353,10 @@
       </c>
       <c r="W82" t="inlineStr"/>
       <c r="X82" t="n">
-        <v>1</v>
+        <v>2002</v>
       </c>
       <c r="Y82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z82" t="n">
         <v>0</v>
@@ -8126,6 +8371,9 @@
         <v>0</v>
       </c>
       <c r="AD82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8200,10 +8448,10 @@
       </c>
       <c r="W83" t="inlineStr"/>
       <c r="X83" t="n">
-        <v>1</v>
+        <v>1996</v>
       </c>
       <c r="Y83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z83" t="n">
         <v>0</v>
@@ -8218,6 +8466,9 @@
         <v>0</v>
       </c>
       <c r="AD83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8292,13 +8543,13 @@
       </c>
       <c r="W84" t="inlineStr"/>
       <c r="X84" t="n">
-        <v>0</v>
+        <v>2003</v>
       </c>
       <c r="Y84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA84" t="n">
         <v>0</v>
@@ -8310,6 +8561,9 @@
         <v>0</v>
       </c>
       <c r="AD84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8384,13 +8638,13 @@
       </c>
       <c r="W85" t="inlineStr"/>
       <c r="X85" t="n">
-        <v>0</v>
+        <v>2006</v>
       </c>
       <c r="Y85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA85" t="n">
         <v>0</v>
@@ -8402,6 +8656,9 @@
         <v>0</v>
       </c>
       <c r="AD85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8478,13 +8735,13 @@
         <v>2635</v>
       </c>
       <c r="X86" t="n">
-        <v>0</v>
+        <v>2021</v>
       </c>
       <c r="Y86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA86" t="n">
         <v>0</v>
@@ -8496,6 +8753,9 @@
         <v>0</v>
       </c>
       <c r="AD86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8570,13 +8830,13 @@
       </c>
       <c r="W87" t="inlineStr"/>
       <c r="X87" t="n">
-        <v>0</v>
+        <v>1989</v>
       </c>
       <c r="Y87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA87" t="n">
         <v>0</v>
@@ -8588,6 +8848,9 @@
         <v>0</v>
       </c>
       <c r="AD87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8664,13 +8927,13 @@
         <v>491</v>
       </c>
       <c r="X88" t="n">
-        <v>0</v>
+        <v>2017</v>
       </c>
       <c r="Y88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA88" t="n">
         <v>0</v>
@@ -8682,6 +8945,9 @@
         <v>0</v>
       </c>
       <c r="AD88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE88" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8758,13 +9024,13 @@
         <v>1023</v>
       </c>
       <c r="X89" t="n">
-        <v>0</v>
+        <v>2015</v>
       </c>
       <c r="Y89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA89" t="n">
         <v>0</v>
@@ -8776,6 +9042,9 @@
         <v>0</v>
       </c>
       <c r="AD89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE89" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8850,13 +9119,13 @@
       </c>
       <c r="W90" t="inlineStr"/>
       <c r="X90" t="n">
-        <v>0</v>
+        <v>1986</v>
       </c>
       <c r="Y90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA90" t="n">
         <v>0</v>
@@ -8868,6 +9137,9 @@
         <v>0</v>
       </c>
       <c r="AD90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8942,10 +9214,10 @@
       </c>
       <c r="W91" t="inlineStr"/>
       <c r="X91" t="n">
-        <v>1</v>
+        <v>1987</v>
       </c>
       <c r="Y91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z91" t="n">
         <v>0</v>
@@ -8960,6 +9232,9 @@
         <v>0</v>
       </c>
       <c r="AD91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE91" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9036,13 +9311,13 @@
         <v>469</v>
       </c>
       <c r="X92" t="n">
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="Y92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA92" t="n">
         <v>0</v>
@@ -9054,6 +9329,9 @@
         <v>0</v>
       </c>
       <c r="AD92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9128,13 +9406,13 @@
       </c>
       <c r="W93" t="inlineStr"/>
       <c r="X93" t="n">
-        <v>0</v>
+        <v>1975</v>
       </c>
       <c r="Y93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA93" t="n">
         <v>0</v>
@@ -9146,6 +9424,9 @@
         <v>0</v>
       </c>
       <c r="AD93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE93" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9222,7 +9503,7 @@
         <v>2283</v>
       </c>
       <c r="X94" t="n">
-        <v>0</v>
+        <v>2011</v>
       </c>
       <c r="Y94" t="n">
         <v>0</v>
@@ -9237,9 +9518,12 @@
         <v>0</v>
       </c>
       <c r="AC94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD94" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE94" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9314,7 +9598,7 @@
       </c>
       <c r="W95" t="inlineStr"/>
       <c r="X95" t="n">
-        <v>0</v>
+        <v>2004</v>
       </c>
       <c r="Y95" t="n">
         <v>0</v>
@@ -9323,15 +9607,18 @@
         <v>0</v>
       </c>
       <c r="AA95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC95" t="n">
         <v>0</v>
       </c>
       <c r="AD95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE95" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9406,13 +9693,13 @@
       </c>
       <c r="W96" t="inlineStr"/>
       <c r="X96" t="n">
-        <v>0</v>
+        <v>1980</v>
       </c>
       <c r="Y96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA96" t="n">
         <v>0</v>
@@ -9424,6 +9711,9 @@
         <v>0</v>
       </c>
       <c r="AD96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE96" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9498,7 +9788,7 @@
       </c>
       <c r="W97" t="inlineStr"/>
       <c r="X97" t="n">
-        <v>0</v>
+        <v>2004</v>
       </c>
       <c r="Y97" t="n">
         <v>0</v>
@@ -9507,15 +9797,18 @@
         <v>0</v>
       </c>
       <c r="AA97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC97" t="n">
         <v>0</v>
       </c>
       <c r="AD97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE97" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9592,10 +9885,10 @@
         <v>1</v>
       </c>
       <c r="X98" t="n">
-        <v>1</v>
+        <v>2018</v>
       </c>
       <c r="Y98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z98" t="n">
         <v>0</v>
@@ -9610,6 +9903,9 @@
         <v>0</v>
       </c>
       <c r="AD98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9684,7 +9980,7 @@
       </c>
       <c r="W99" t="inlineStr"/>
       <c r="X99" t="n">
-        <v>0</v>
+        <v>1984</v>
       </c>
       <c r="Y99" t="n">
         <v>0</v>
@@ -9693,15 +9989,18 @@
         <v>0</v>
       </c>
       <c r="AA99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC99" t="n">
         <v>0</v>
       </c>
       <c r="AD99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE99" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9776,13 +10075,13 @@
       </c>
       <c r="W100" t="inlineStr"/>
       <c r="X100" t="n">
-        <v>0</v>
+        <v>1976</v>
       </c>
       <c r="Y100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA100" t="n">
         <v>0</v>
@@ -9794,6 +10093,9 @@
         <v>0</v>
       </c>
       <c r="AD100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE100" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9870,7 +10172,7 @@
         <v>1011</v>
       </c>
       <c r="X101" t="n">
-        <v>0</v>
+        <v>2009</v>
       </c>
       <c r="Y101" t="n">
         <v>0</v>
@@ -9879,15 +10181,18 @@
         <v>0</v>
       </c>
       <c r="AA101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC101" t="n">
         <v>0</v>
       </c>
       <c r="AD101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE101" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9964,10 +10269,10 @@
         <v>1644</v>
       </c>
       <c r="X102" t="n">
-        <v>1</v>
+        <v>2010</v>
       </c>
       <c r="Y102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z102" t="n">
         <v>0</v>
@@ -9982,6 +10287,9 @@
         <v>0</v>
       </c>
       <c r="AD102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE102" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10056,13 +10364,13 @@
       </c>
       <c r="W103" t="inlineStr"/>
       <c r="X103" t="n">
-        <v>0</v>
+        <v>1996</v>
       </c>
       <c r="Y103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA103" t="n">
         <v>0</v>
@@ -10074,6 +10382,9 @@
         <v>0</v>
       </c>
       <c r="AD103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE103" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10148,7 +10459,7 @@
       </c>
       <c r="W104" t="inlineStr"/>
       <c r="X104" t="n">
-        <v>0</v>
+        <v>2006</v>
       </c>
       <c r="Y104" t="n">
         <v>0</v>
@@ -10157,15 +10468,18 @@
         <v>0</v>
       </c>
       <c r="AA104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC104" t="n">
         <v>0</v>
       </c>
       <c r="AD104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE104" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10242,10 +10556,10 @@
         <v>983</v>
       </c>
       <c r="X105" t="n">
-        <v>1</v>
+        <v>2009</v>
       </c>
       <c r="Y105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z105" t="n">
         <v>0</v>
@@ -10260,6 +10574,9 @@
         <v>0</v>
       </c>
       <c r="AD105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE105" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10334,7 +10651,7 @@
       </c>
       <c r="W106" t="inlineStr"/>
       <c r="X106" t="n">
-        <v>0</v>
+        <v>2006</v>
       </c>
       <c r="Y106" t="n">
         <v>0</v>
@@ -10343,15 +10660,18 @@
         <v>0</v>
       </c>
       <c r="AA106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC106" t="n">
         <v>0</v>
       </c>
       <c r="AD106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE106" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10428,10 +10748,10 @@
         <v>0</v>
       </c>
       <c r="X107" t="n">
-        <v>1</v>
+        <v>2009</v>
       </c>
       <c r="Y107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z107" t="n">
         <v>0</v>
@@ -10446,6 +10766,9 @@
         <v>0</v>
       </c>
       <c r="AD107" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE107" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10520,10 +10843,10 @@
       </c>
       <c r="W108" t="inlineStr"/>
       <c r="X108" t="n">
-        <v>1</v>
+        <v>2007</v>
       </c>
       <c r="Y108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z108" t="n">
         <v>0</v>
@@ -10538,6 +10861,9 @@
         <v>0</v>
       </c>
       <c r="AD108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE108" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10614,13 +10940,13 @@
         <v>1094</v>
       </c>
       <c r="X109" t="n">
-        <v>0</v>
+        <v>2014</v>
       </c>
       <c r="Y109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA109" t="n">
         <v>0</v>
@@ -10632,6 +10958,9 @@
         <v>0</v>
       </c>
       <c r="AD109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE109" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10706,7 +11035,7 @@
       </c>
       <c r="W110" t="inlineStr"/>
       <c r="X110" t="n">
-        <v>0</v>
+        <v>1999</v>
       </c>
       <c r="Y110" t="n">
         <v>0</v>
@@ -10718,12 +11047,15 @@
         <v>0</v>
       </c>
       <c r="AB110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD110" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE110" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10798,13 +11130,13 @@
       </c>
       <c r="W111" t="inlineStr"/>
       <c r="X111" t="n">
-        <v>0</v>
+        <v>1983</v>
       </c>
       <c r="Y111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA111" t="n">
         <v>0</v>
@@ -10816,6 +11148,9 @@
         <v>0</v>
       </c>
       <c r="AD111" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE111" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10890,13 +11225,13 @@
       </c>
       <c r="W112" t="inlineStr"/>
       <c r="X112" t="n">
-        <v>0</v>
+        <v>1997</v>
       </c>
       <c r="Y112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA112" t="n">
         <v>0</v>
@@ -10908,6 +11243,9 @@
         <v>0</v>
       </c>
       <c r="AD112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE112" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10984,13 +11322,13 @@
         <v>478</v>
       </c>
       <c r="X113" t="n">
-        <v>0</v>
+        <v>2012</v>
       </c>
       <c r="Y113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA113" t="n">
         <v>0</v>
@@ -11002,6 +11340,9 @@
         <v>0</v>
       </c>
       <c r="AD113" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE113" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11076,10 +11417,10 @@
       </c>
       <c r="W114" t="inlineStr"/>
       <c r="X114" t="n">
-        <v>1</v>
+        <v>1999</v>
       </c>
       <c r="Y114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z114" t="n">
         <v>0</v>
@@ -11094,6 +11435,9 @@
         <v>0</v>
       </c>
       <c r="AD114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE114" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11170,13 +11514,13 @@
         <v>362</v>
       </c>
       <c r="X115" t="n">
-        <v>0</v>
+        <v>2018</v>
       </c>
       <c r="Y115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA115" t="n">
         <v>0</v>
@@ -11188,6 +11532,9 @@
         <v>0</v>
       </c>
       <c r="AD115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE115" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11262,7 +11609,7 @@
       </c>
       <c r="W116" t="inlineStr"/>
       <c r="X116" t="n">
-        <v>0</v>
+        <v>1942</v>
       </c>
       <c r="Y116" t="n">
         <v>0</v>
@@ -11280,6 +11627,9 @@
         <v>0</v>
       </c>
       <c r="AD116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE116" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11354,10 +11704,10 @@
       </c>
       <c r="W117" t="inlineStr"/>
       <c r="X117" t="n">
-        <v>1</v>
+        <v>1986</v>
       </c>
       <c r="Y117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z117" t="n">
         <v>0</v>
@@ -11372,6 +11722,9 @@
         <v>0</v>
       </c>
       <c r="AD117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE117" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11446,7 +11799,7 @@
       </c>
       <c r="W118" t="inlineStr"/>
       <c r="X118" t="n">
-        <v>0</v>
+        <v>1985</v>
       </c>
       <c r="Y118" t="n">
         <v>0</v>
@@ -11455,15 +11808,18 @@
         <v>0</v>
       </c>
       <c r="AA118" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC118" t="n">
         <v>0</v>
       </c>
       <c r="AD118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE118" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11538,10 +11894,10 @@
       </c>
       <c r="W119" t="inlineStr"/>
       <c r="X119" t="n">
-        <v>1</v>
+        <v>1986</v>
       </c>
       <c r="Y119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z119" t="n">
         <v>0</v>
@@ -11556,6 +11912,9 @@
         <v>0</v>
       </c>
       <c r="AD119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE119" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11630,13 +11989,13 @@
       </c>
       <c r="W120" t="inlineStr"/>
       <c r="X120" t="n">
-        <v>0</v>
+        <v>1992</v>
       </c>
       <c r="Y120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA120" t="n">
         <v>0</v>
@@ -11648,6 +12007,9 @@
         <v>0</v>
       </c>
       <c r="AD120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE120" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11724,13 +12086,13 @@
         <v>731</v>
       </c>
       <c r="X121" t="n">
-        <v>0</v>
+        <v>2014</v>
       </c>
       <c r="Y121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA121" t="n">
         <v>0</v>
@@ -11742,6 +12104,9 @@
         <v>0</v>
       </c>
       <c r="AD121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE121" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11816,13 +12181,13 @@
       </c>
       <c r="W122" t="inlineStr"/>
       <c r="X122" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="Y122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA122" t="n">
         <v>0</v>
@@ -11834,6 +12199,9 @@
         <v>0</v>
       </c>
       <c r="AD122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE122" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11908,7 +12276,7 @@
       </c>
       <c r="W123" t="inlineStr"/>
       <c r="X123" t="n">
-        <v>0</v>
+        <v>1993</v>
       </c>
       <c r="Y123" t="n">
         <v>0</v>
@@ -11917,15 +12285,18 @@
         <v>0</v>
       </c>
       <c r="AA123" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC123" t="n">
         <v>0</v>
       </c>
       <c r="AD123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE123" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12000,13 +12371,13 @@
       </c>
       <c r="W124" t="inlineStr"/>
       <c r="X124" t="n">
-        <v>0</v>
+        <v>1968</v>
       </c>
       <c r="Y124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA124" t="n">
         <v>0</v>
@@ -12018,6 +12389,9 @@
         <v>0</v>
       </c>
       <c r="AD124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE124" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12092,13 +12466,13 @@
       </c>
       <c r="W125" t="inlineStr"/>
       <c r="X125" t="n">
-        <v>0</v>
+        <v>1995</v>
       </c>
       <c r="Y125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA125" t="n">
         <v>0</v>
@@ -12110,6 +12484,9 @@
         <v>0</v>
       </c>
       <c r="AD125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE125" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12184,13 +12561,13 @@
       </c>
       <c r="W126" t="inlineStr"/>
       <c r="X126" t="n">
-        <v>0</v>
+        <v>2006</v>
       </c>
       <c r="Y126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA126" t="n">
         <v>0</v>
@@ -12202,6 +12579,9 @@
         <v>0</v>
       </c>
       <c r="AD126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE126" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12278,16 +12658,16 @@
         <v>2</v>
       </c>
       <c r="X127" t="n">
-        <v>0</v>
+        <v>2017</v>
       </c>
       <c r="Y127" t="n">
         <v>0</v>
       </c>
       <c r="Z127" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB127" t="n">
         <v>0</v>
@@ -12296,6 +12676,9 @@
         <v>0</v>
       </c>
       <c r="AD127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE127" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12370,13 +12753,13 @@
       </c>
       <c r="W128" t="inlineStr"/>
       <c r="X128" t="n">
-        <v>0</v>
+        <v>1991</v>
       </c>
       <c r="Y128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA128" t="n">
         <v>0</v>
@@ -12388,6 +12771,9 @@
         <v>0</v>
       </c>
       <c r="AD128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE128" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12462,13 +12848,13 @@
       </c>
       <c r="W129" t="inlineStr"/>
       <c r="X129" t="n">
-        <v>0</v>
+        <v>2005</v>
       </c>
       <c r="Y129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA129" t="n">
         <v>0</v>
@@ -12480,6 +12866,9 @@
         <v>0</v>
       </c>
       <c r="AD129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE129" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12554,7 +12943,7 @@
       </c>
       <c r="W130" t="inlineStr"/>
       <c r="X130" t="n">
-        <v>0</v>
+        <v>1996</v>
       </c>
       <c r="Y130" t="n">
         <v>0</v>
@@ -12563,15 +12952,18 @@
         <v>0</v>
       </c>
       <c r="AA130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC130" t="n">
         <v>0</v>
       </c>
       <c r="AD130" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE130" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12648,10 +13040,10 @@
         <v>8</v>
       </c>
       <c r="X131" t="n">
-        <v>1</v>
+        <v>2019</v>
       </c>
       <c r="Y131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z131" t="n">
         <v>0</v>
@@ -12666,6 +13058,9 @@
         <v>0</v>
       </c>
       <c r="AD131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE131" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12740,7 +13135,7 @@
       </c>
       <c r="W132" t="inlineStr"/>
       <c r="X132" t="n">
-        <v>0</v>
+        <v>2007</v>
       </c>
       <c r="Y132" t="n">
         <v>0</v>
@@ -12749,15 +13144,18 @@
         <v>0</v>
       </c>
       <c r="AA132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC132" t="n">
         <v>0</v>
       </c>
       <c r="AD132" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE132" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12832,13 +13230,13 @@
       </c>
       <c r="W133" t="inlineStr"/>
       <c r="X133" t="n">
-        <v>0</v>
+        <v>2007</v>
       </c>
       <c r="Y133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA133" t="n">
         <v>0</v>
@@ -12850,6 +13248,9 @@
         <v>0</v>
       </c>
       <c r="AD133" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE133" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12924,16 +13325,16 @@
         <v>3153</v>
       </c>
       <c r="X134" t="n">
-        <v>0</v>
+        <v>2017</v>
       </c>
       <c r="Y134" t="n">
         <v>0</v>
       </c>
       <c r="Z134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB134" t="n">
         <v>0</v>
@@ -12942,6 +13343,9 @@
         <v>0</v>
       </c>
       <c r="AD134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE134" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>